<commit_message>
Update specification et Maj du planning
</commit_message>
<xml_diff>
--- a/Documentation/Planification.xlsx
+++ b/Documentation/Planification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/371c2caacf93074d/Documents/HEIG/TB Driver Brushless/TB-Driver-Brushless/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="665" documentId="8_{CB7147DC-5DFD-4F3C-85F9-1BD4040EC95A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{72A4C906-8740-4162-B7D1-F498055E2350}"/>
+  <xr:revisionPtr revIDLastSave="674" documentId="8_{CB7147DC-5DFD-4F3C-85F9-1BD4040EC95A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8368EFC5-1C7D-4D68-A05C-000650339940}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{E4DCEC7E-A84B-4A69-AC68-472FA9C158BB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E4DCEC7E-A84B-4A69-AC68-472FA9C158BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -836,95 +836,95 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -942,36 +942,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1297,8 +1267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09FBCC03-12B2-4877-A171-7A10D6B76BA3}">
   <dimension ref="A1:AB48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+    <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1319,10 +1289,10 @@
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="36"/>
+      <c r="C1" s="62"/>
       <c r="D1" s="14" t="s">
         <v>35</v>
       </c>
@@ -1389,10 +1359,10 @@
       <c r="Y1" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="Z1" s="50" t="s">
+      <c r="Z1" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="AA1" s="56" t="s">
+      <c r="AA1" s="51" t="s">
         <v>87</v>
       </c>
       <c r="AB1" s="15" t="s">
@@ -1403,10 +1373,10 @@
       <c r="A2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="35"/>
+      <c r="C2" s="61"/>
       <c r="D2" s="1"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -1429,7 +1399,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
-      <c r="Z2" s="51"/>
+      <c r="Z2" s="46"/>
       <c r="AA2" s="1"/>
       <c r="AB2" s="3"/>
     </row>
@@ -1444,10 +1414,10 @@
       <c r="D3" s="4">
         <v>5</v>
       </c>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="47"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="42"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
@@ -1465,7 +1435,7 @@
       <c r="W3" s="5"/>
       <c r="X3" s="5"/>
       <c r="Y3" s="5"/>
-      <c r="Z3" s="52"/>
+      <c r="Z3" s="47"/>
       <c r="AA3" s="4">
         <f>SUM(E3:Z3)</f>
         <v>0</v>
@@ -1486,10 +1456,10 @@
       <c r="D4" s="4">
         <v>5</v>
       </c>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="47"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="42"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
@@ -1507,7 +1477,7 @@
       <c r="W4" s="5"/>
       <c r="X4" s="5"/>
       <c r="Y4" s="5"/>
-      <c r="Z4" s="52"/>
+      <c r="Z4" s="47"/>
       <c r="AA4" s="4">
         <f>SUM(E4:Z4)</f>
         <v>0</v>
@@ -1530,8 +1500,8 @@
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="47"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="42"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
@@ -1549,7 +1519,7 @@
       <c r="W5" s="5"/>
       <c r="X5" s="5"/>
       <c r="Y5" s="5"/>
-      <c r="Z5" s="52"/>
+      <c r="Z5" s="47"/>
       <c r="AA5" s="4">
         <f>SUM(F5:Z5)</f>
         <v>0</v>
@@ -1570,15 +1540,19 @@
       <c r="D6" s="7">
         <v>15</v>
       </c>
-      <c r="E6" s="58"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="58"/>
-      <c r="L6" s="58"/>
-      <c r="M6" s="58"/>
+      <c r="E6" s="53">
+        <v>1.5</v>
+      </c>
+      <c r="F6" s="43">
+        <v>5</v>
+      </c>
+      <c r="G6" s="43"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
+      <c r="L6" s="53"/>
+      <c r="M6" s="53"/>
       <c r="N6" s="8"/>
       <c r="O6" s="8"/>
       <c r="P6" s="8"/>
@@ -1591,24 +1565,24 @@
       <c r="W6" s="8"/>
       <c r="X6" s="8"/>
       <c r="Y6" s="8"/>
-      <c r="Z6" s="53"/>
+      <c r="Z6" s="48"/>
       <c r="AA6" s="4">
         <f>SUM(E6:Z6)</f>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="AB6" s="6">
         <f>D6-AA6</f>
-        <v>15</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="35"/>
+      <c r="C7" s="61"/>
       <c r="D7" s="1"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -1631,7 +1605,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
-      <c r="Z7" s="51"/>
+      <c r="Z7" s="46"/>
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
     </row>
@@ -1648,13 +1622,13 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="26"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="59"/>
-      <c r="L8" s="44"/>
-      <c r="N8" s="44"/>
-      <c r="O8" s="44"/>
-      <c r="P8" s="44"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="39"/>
+      <c r="N8" s="39"/>
+      <c r="O8" s="39"/>
+      <c r="P8" s="39"/>
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
       <c r="S8" s="5"/>
@@ -1664,7 +1638,7 @@
       <c r="W8" s="5"/>
       <c r="X8" s="5"/>
       <c r="Y8" s="5"/>
-      <c r="Z8" s="52"/>
+      <c r="Z8" s="47"/>
       <c r="AA8" s="4">
         <f>SUM(E8:Z8)</f>
         <v>0</v>
@@ -1687,10 +1661,10 @@
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="26"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="60"/>
-      <c r="L9" s="44"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="55"/>
+      <c r="K9" s="55"/>
+      <c r="L9" s="39"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
@@ -1703,7 +1677,7 @@
       <c r="W9" s="5"/>
       <c r="X9" s="5"/>
       <c r="Y9" s="5"/>
-      <c r="Z9" s="52"/>
+      <c r="Z9" s="47"/>
       <c r="AA9" s="4">
         <f>SUM(F9:Z9)</f>
         <v>0</v>
@@ -1726,10 +1700,10 @@
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="28"/>
-      <c r="I10" s="61"/>
-      <c r="J10" s="61"/>
-      <c r="K10" s="61"/>
-      <c r="L10" s="58"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="53"/>
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
       <c r="O10" s="8"/>
@@ -1743,7 +1717,7 @@
       <c r="W10" s="8"/>
       <c r="X10" s="8"/>
       <c r="Y10" s="8"/>
-      <c r="Z10" s="53"/>
+      <c r="Z10" s="48"/>
       <c r="AA10" s="4">
         <f>SUM(E10:Z10)</f>
         <v>0</v>
@@ -1757,10 +1731,10 @@
       <c r="A11" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="35"/>
+      <c r="C11" s="61"/>
       <c r="D11" s="1"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -1783,7 +1757,7 @@
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
-      <c r="Z11" s="51"/>
+      <c r="Z11" s="46"/>
       <c r="AA11" s="1">
         <f>SUM(E11:Z11)</f>
         <v>0</v>
@@ -1809,7 +1783,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
-      <c r="L12" s="45"/>
+      <c r="L12" s="40"/>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
@@ -1821,7 +1795,7 @@
       <c r="W12" s="5"/>
       <c r="X12" s="5"/>
       <c r="Y12" s="5"/>
-      <c r="Z12" s="52"/>
+      <c r="Z12" s="47"/>
       <c r="AA12" s="4"/>
       <c r="AB12" s="6"/>
     </row>
@@ -1842,7 +1816,7 @@
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
-      <c r="M13" s="45"/>
+      <c r="M13" s="40"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
@@ -1853,7 +1827,7 @@
       <c r="W13" s="5"/>
       <c r="X13" s="5"/>
       <c r="Y13" s="5"/>
-      <c r="Z13" s="52"/>
+      <c r="Z13" s="47"/>
       <c r="AA13" s="4"/>
       <c r="AB13" s="6"/>
     </row>
@@ -1874,9 +1848,9 @@
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
-      <c r="M14" s="45"/>
-      <c r="N14" s="45"/>
-      <c r="O14" s="45"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="40"/>
+      <c r="O14" s="40"/>
       <c r="P14" s="5"/>
       <c r="S14" s="5"/>
       <c r="T14" s="5"/>
@@ -1885,14 +1859,14 @@
       <c r="W14" s="5"/>
       <c r="X14" s="5"/>
       <c r="Y14" s="5"/>
-      <c r="Z14" s="52"/>
+      <c r="Z14" s="47"/>
       <c r="AA14" s="4"/>
       <c r="AB14" s="6"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" s="34"/>
       <c r="B15" s="23"/>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="35" t="s">
         <v>96</v>
       </c>
       <c r="D15" s="4">
@@ -1908,7 +1882,7 @@
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
-      <c r="O15" s="45"/>
+      <c r="O15" s="40"/>
       <c r="P15" s="5"/>
       <c r="S15" s="5"/>
       <c r="T15" s="5"/>
@@ -1917,14 +1891,14 @@
       <c r="W15" s="5"/>
       <c r="X15" s="5"/>
       <c r="Y15" s="5"/>
-      <c r="Z15" s="52"/>
+      <c r="Z15" s="47"/>
       <c r="AA15" s="4"/>
       <c r="AB15" s="6"/>
     </row>
     <row r="16" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="20"/>
       <c r="B16" s="21"/>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="35" t="s">
         <v>97</v>
       </c>
       <c r="D16" s="7">
@@ -1941,7 +1915,7 @@
       <c r="M16" s="8"/>
       <c r="N16" s="8"/>
       <c r="O16" s="8"/>
-      <c r="P16" s="48"/>
+      <c r="P16" s="43"/>
       <c r="S16" s="8"/>
       <c r="T16" s="8"/>
       <c r="U16" s="28"/>
@@ -1949,7 +1923,7 @@
       <c r="W16" s="8"/>
       <c r="X16" s="8"/>
       <c r="Y16" s="8"/>
-      <c r="Z16" s="53"/>
+      <c r="Z16" s="48"/>
       <c r="AA16" s="4">
         <f>SUM(E16:Z16)</f>
         <v>0</v>
@@ -1963,10 +1937,10 @@
       <c r="A17" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="35"/>
+      <c r="C17" s="61"/>
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -1989,7 +1963,7 @@
       <c r="W17" s="2"/>
       <c r="X17" s="2"/>
       <c r="Y17" s="2"/>
-      <c r="Z17" s="51"/>
+      <c r="Z17" s="46"/>
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
     </row>
@@ -2016,7 +1990,7 @@
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
-      <c r="Q18" s="45"/>
+      <c r="Q18" s="40"/>
       <c r="R18" s="5"/>
       <c r="S18" s="5"/>
       <c r="T18" s="5"/>
@@ -2025,7 +1999,7 @@
       <c r="W18" s="5"/>
       <c r="X18" s="5"/>
       <c r="Y18" s="5"/>
-      <c r="Z18" s="52"/>
+      <c r="Z18" s="47"/>
       <c r="AA18" s="4">
         <f>SUM(E18:Z18)</f>
         <v>0</v>
@@ -2046,9 +2020,7 @@
       <c r="D19" s="4">
         <v>10</v>
       </c>
-      <c r="E19" s="5">
-        <v>1.5</v>
-      </c>
+      <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="26"/>
@@ -2060,7 +2032,7 @@
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
-      <c r="Q19" s="45"/>
+      <c r="Q19" s="40"/>
       <c r="R19" s="5"/>
       <c r="S19" s="5"/>
       <c r="T19" s="5"/>
@@ -2069,14 +2041,14 @@
       <c r="W19" s="5"/>
       <c r="X19" s="5"/>
       <c r="Y19" s="5"/>
-      <c r="Z19" s="52"/>
+      <c r="Z19" s="47"/>
       <c r="AA19" s="4">
         <f>SUM(E19:Z19)</f>
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="AB19" s="4">
         <f>D19-AA19</f>
-        <v>8.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -2102,7 +2074,7 @@
       <c r="N20" s="8"/>
       <c r="O20" s="8"/>
       <c r="P20" s="8"/>
-      <c r="Q20" s="48"/>
+      <c r="Q20" s="43"/>
       <c r="R20" s="8"/>
       <c r="S20" s="8"/>
       <c r="T20" s="8"/>
@@ -2111,7 +2083,7 @@
       <c r="W20" s="8"/>
       <c r="X20" s="8"/>
       <c r="Y20" s="8"/>
-      <c r="Z20" s="53"/>
+      <c r="Z20" s="48"/>
       <c r="AA20" s="4">
         <f>SUM(E20:Z20)</f>
         <v>0</v>
@@ -2125,20 +2097,20 @@
       <c r="A21" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="35" t="s">
+      <c r="B21" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="35"/>
+      <c r="C21" s="61"/>
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="31"/>
       <c r="I21" s="2"/>
-      <c r="J21" s="62"/>
-      <c r="K21" s="62"/>
-      <c r="L21" s="44"/>
-      <c r="M21" s="62"/>
+      <c r="J21" s="57"/>
+      <c r="K21" s="57"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="57"/>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
@@ -2151,7 +2123,7 @@
       <c r="W21" s="2"/>
       <c r="X21" s="2"/>
       <c r="Y21" s="2"/>
-      <c r="Z21" s="51"/>
+      <c r="Z21" s="46"/>
       <c r="AA21" s="1"/>
       <c r="AB21" s="6"/>
     </row>
@@ -2171,29 +2143,29 @@
       <c r="G22" s="5"/>
       <c r="H22" s="26"/>
       <c r="I22" s="5"/>
-      <c r="J22" s="44"/>
-      <c r="K22" s="44"/>
-      <c r="L22" s="44"/>
-      <c r="M22" s="44"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="39"/>
+      <c r="L22" s="39"/>
+      <c r="M22" s="39"/>
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
       <c r="Q22" s="5"/>
-      <c r="R22" s="45"/>
-      <c r="S22" s="45"/>
-      <c r="T22" s="44"/>
+      <c r="R22" s="40"/>
+      <c r="S22" s="40"/>
+      <c r="T22" s="39"/>
       <c r="U22" s="26"/>
       <c r="V22" s="5"/>
       <c r="W22" s="5"/>
       <c r="X22" s="5"/>
       <c r="Y22" s="5"/>
-      <c r="Z22" s="52"/>
+      <c r="Z22" s="47"/>
       <c r="AA22" s="4">
-        <f>SUM(E22:Z22)</f>
+        <f t="shared" ref="AA22:AA31" si="0">SUM(E22:Z22)</f>
         <v>0</v>
       </c>
       <c r="AB22" s="6">
-        <f>D22-AA22</f>
+        <f t="shared" ref="AB22:AB31" si="1">D22-AA22</f>
         <v>20</v>
       </c>
     </row>
@@ -2213,29 +2185,29 @@
       <c r="G23" s="5"/>
       <c r="H23" s="26"/>
       <c r="I23" s="5"/>
-      <c r="J23" s="44"/>
-      <c r="K23" s="44"/>
-      <c r="L23" s="44"/>
-      <c r="M23" s="44"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="39"/>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
       <c r="P23" s="5"/>
       <c r="Q23" s="5"/>
       <c r="R23" s="5"/>
-      <c r="S23" s="45"/>
-      <c r="T23" s="45"/>
+      <c r="S23" s="40"/>
+      <c r="T23" s="40"/>
       <c r="U23" s="26"/>
       <c r="V23" s="5"/>
       <c r="W23" s="5"/>
       <c r="X23" s="5"/>
       <c r="Y23" s="5"/>
-      <c r="Z23" s="52"/>
+      <c r="Z23" s="47"/>
       <c r="AA23" s="4">
-        <f>SUM(E23:Z23)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB23" s="6">
-        <f>D23-AA23</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
     </row>
@@ -2257,27 +2229,27 @@
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
-      <c r="L24" s="44"/>
-      <c r="M24" s="44"/>
-      <c r="N24" s="44"/>
-      <c r="O24" s="44"/>
-      <c r="P24" s="44"/>
-      <c r="Q24" s="44"/>
-      <c r="R24" s="44"/>
-      <c r="S24" s="44"/>
-      <c r="T24" s="45"/>
-      <c r="U24" s="47"/>
+      <c r="L24" s="39"/>
+      <c r="M24" s="39"/>
+      <c r="N24" s="39"/>
+      <c r="O24" s="39"/>
+      <c r="P24" s="39"/>
+      <c r="Q24" s="39"/>
+      <c r="R24" s="39"/>
+      <c r="S24" s="39"/>
+      <c r="T24" s="40"/>
+      <c r="U24" s="42"/>
       <c r="V24" s="5"/>
       <c r="W24" s="5"/>
       <c r="X24" s="5"/>
       <c r="Y24" s="5"/>
-      <c r="Z24" s="52"/>
+      <c r="Z24" s="47"/>
       <c r="AA24" s="4">
-        <f>SUM(E24:Z24)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB24" s="6">
-        <f>D24-AA24</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
     </row>
@@ -2299,27 +2271,27 @@
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
-      <c r="L25" s="44"/>
-      <c r="M25" s="44"/>
-      <c r="N25" s="44"/>
-      <c r="O25" s="44"/>
-      <c r="P25" s="44"/>
-      <c r="Q25" s="44"/>
-      <c r="R25" s="44"/>
-      <c r="S25" s="44"/>
-      <c r="T25" s="45"/>
-      <c r="U25" s="47"/>
+      <c r="L25" s="39"/>
+      <c r="M25" s="39"/>
+      <c r="N25" s="39"/>
+      <c r="O25" s="39"/>
+      <c r="P25" s="39"/>
+      <c r="Q25" s="39"/>
+      <c r="R25" s="39"/>
+      <c r="S25" s="39"/>
+      <c r="T25" s="40"/>
+      <c r="U25" s="42"/>
       <c r="V25" s="5"/>
       <c r="W25" s="5"/>
       <c r="X25" s="5"/>
       <c r="Y25" s="5"/>
-      <c r="Z25" s="52"/>
+      <c r="Z25" s="47"/>
       <c r="AA25" s="4">
-        <f>SUM(E25:Z25)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB25" s="6">
-        <f>D25-AA25</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
     </row>
@@ -2341,27 +2313,27 @@
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
-      <c r="L26" s="44"/>
-      <c r="M26" s="44"/>
-      <c r="N26" s="44"/>
-      <c r="O26" s="44"/>
-      <c r="P26" s="44"/>
-      <c r="Q26" s="44"/>
-      <c r="R26" s="44"/>
-      <c r="S26" s="44"/>
+      <c r="L26" s="39"/>
+      <c r="M26" s="39"/>
+      <c r="N26" s="39"/>
+      <c r="O26" s="39"/>
+      <c r="P26" s="39"/>
+      <c r="Q26" s="39"/>
+      <c r="R26" s="39"/>
+      <c r="S26" s="39"/>
       <c r="T26" s="5"/>
-      <c r="U26" s="47"/>
-      <c r="V26" s="45"/>
+      <c r="U26" s="42"/>
+      <c r="V26" s="40"/>
       <c r="W26" s="5"/>
       <c r="X26" s="5"/>
       <c r="Y26" s="5"/>
-      <c r="Z26" s="52"/>
+      <c r="Z26" s="47"/>
       <c r="AA26" s="4">
-        <f>SUM(E26:Z26)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB26" s="6">
-        <f>D26-AA26</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
     </row>
@@ -2383,27 +2355,27 @@
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
-      <c r="L27" s="44"/>
-      <c r="M27" s="44"/>
-      <c r="N27" s="44"/>
-      <c r="O27" s="44"/>
-      <c r="P27" s="44"/>
-      <c r="Q27" s="44"/>
-      <c r="R27" s="44"/>
-      <c r="S27" s="44"/>
+      <c r="L27" s="39"/>
+      <c r="M27" s="39"/>
+      <c r="N27" s="39"/>
+      <c r="O27" s="39"/>
+      <c r="P27" s="39"/>
+      <c r="Q27" s="39"/>
+      <c r="R27" s="39"/>
+      <c r="S27" s="39"/>
       <c r="T27" s="5"/>
-      <c r="U27" s="47"/>
-      <c r="V27" s="45"/>
+      <c r="U27" s="42"/>
+      <c r="V27" s="40"/>
       <c r="W27" s="5"/>
       <c r="X27" s="5"/>
       <c r="Y27" s="5"/>
-      <c r="Z27" s="52"/>
+      <c r="Z27" s="47"/>
       <c r="AA27" s="4">
-        <f>SUM(E27:Z27)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB27" s="6">
-        <f>D27-AA27</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
@@ -2425,27 +2397,27 @@
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
-      <c r="L28" s="44"/>
-      <c r="M28" s="44"/>
-      <c r="N28" s="44"/>
-      <c r="O28" s="44"/>
-      <c r="P28" s="44"/>
-      <c r="Q28" s="44"/>
-      <c r="R28" s="44"/>
-      <c r="S28" s="44"/>
+      <c r="L28" s="39"/>
+      <c r="M28" s="39"/>
+      <c r="N28" s="39"/>
+      <c r="O28" s="39"/>
+      <c r="P28" s="39"/>
+      <c r="Q28" s="39"/>
+      <c r="R28" s="39"/>
+      <c r="S28" s="39"/>
       <c r="T28" s="5"/>
       <c r="U28" s="26"/>
-      <c r="V28" s="45"/>
-      <c r="W28" s="45"/>
+      <c r="V28" s="40"/>
+      <c r="W28" s="40"/>
       <c r="X28" s="5"/>
       <c r="Y28" s="5"/>
-      <c r="Z28" s="52"/>
+      <c r="Z28" s="47"/>
       <c r="AA28" s="4">
-        <f>SUM(E28:Z28)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB28" s="6">
-        <f>D28-AA28</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -2467,27 +2439,27 @@
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
-      <c r="L29" s="44"/>
-      <c r="M29" s="44"/>
-      <c r="N29" s="44"/>
-      <c r="O29" s="44"/>
-      <c r="P29" s="44"/>
-      <c r="Q29" s="44"/>
-      <c r="R29" s="44"/>
-      <c r="S29" s="44"/>
+      <c r="L29" s="39"/>
+      <c r="M29" s="39"/>
+      <c r="N29" s="39"/>
+      <c r="O29" s="39"/>
+      <c r="P29" s="39"/>
+      <c r="Q29" s="39"/>
+      <c r="R29" s="39"/>
+      <c r="S29" s="39"/>
       <c r="T29" s="5"/>
       <c r="U29" s="26"/>
       <c r="V29" s="5"/>
-      <c r="W29" s="45"/>
-      <c r="X29" s="45"/>
+      <c r="W29" s="40"/>
+      <c r="X29" s="40"/>
       <c r="Y29" s="5"/>
-      <c r="Z29" s="52"/>
+      <c r="Z29" s="47"/>
       <c r="AA29" s="4">
-        <f>SUM(E29:Z29)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB29" s="6">
-        <f>D29-AA29</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
@@ -2495,7 +2467,7 @@
       <c r="A30" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="B30" s="37"/>
+      <c r="B30" s="35"/>
       <c r="C30" s="22" t="s">
         <v>91</v>
       </c>
@@ -2509,27 +2481,27 @@
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
-      <c r="L30" s="58"/>
-      <c r="M30" s="58"/>
-      <c r="N30" s="58"/>
-      <c r="O30" s="58"/>
-      <c r="P30" s="58"/>
-      <c r="Q30" s="58"/>
-      <c r="R30" s="58"/>
-      <c r="S30" s="58"/>
+      <c r="L30" s="53"/>
+      <c r="M30" s="53"/>
+      <c r="N30" s="53"/>
+      <c r="O30" s="53"/>
+      <c r="P30" s="53"/>
+      <c r="Q30" s="53"/>
+      <c r="R30" s="53"/>
+      <c r="S30" s="53"/>
       <c r="T30" s="8"/>
       <c r="U30" s="28"/>
-      <c r="V30" s="48"/>
-      <c r="W30" s="48"/>
-      <c r="X30" s="48"/>
-      <c r="Y30" s="48"/>
-      <c r="Z30" s="55"/>
+      <c r="V30" s="43"/>
+      <c r="W30" s="43"/>
+      <c r="X30" s="43"/>
+      <c r="Y30" s="43"/>
+      <c r="Z30" s="50"/>
       <c r="AA30" s="4">
-        <f>SUM(E30:Z30)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB30" s="6">
-        <f>D30-AA30</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
     </row>
@@ -2537,10 +2509,10 @@
       <c r="A31" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="35" t="s">
+      <c r="B31" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="35"/>
+      <c r="C31" s="61"/>
       <c r="D31" s="1"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
@@ -2563,13 +2535,13 @@
       <c r="W31" s="2"/>
       <c r="X31" s="2"/>
       <c r="Y31" s="2"/>
-      <c r="Z31" s="51"/>
+      <c r="Z31" s="46"/>
       <c r="AA31" s="1">
-        <f>SUM(E31:Z31)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB31" s="1">
-        <f>D31-AA31</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2602,8 +2574,8 @@
       <c r="V32" s="5"/>
       <c r="W32" s="5"/>
       <c r="X32" s="5"/>
-      <c r="Y32" s="45"/>
-      <c r="Z32" s="54"/>
+      <c r="Y32" s="40"/>
+      <c r="Z32" s="49"/>
       <c r="AA32" s="4"/>
       <c r="AB32" s="4"/>
     </row>
@@ -2636,8 +2608,8 @@
       <c r="V33" s="5"/>
       <c r="W33" s="5"/>
       <c r="X33" s="5"/>
-      <c r="Y33" s="45"/>
-      <c r="Z33" s="54"/>
+      <c r="Y33" s="40"/>
+      <c r="Z33" s="49"/>
       <c r="AA33" s="4"/>
       <c r="AB33" s="4"/>
     </row>
@@ -2645,10 +2617,10 @@
       <c r="A34" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="35" t="s">
+      <c r="B34" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="35"/>
+      <c r="C34" s="61"/>
       <c r="D34" s="1"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
@@ -2671,7 +2643,7 @@
       <c r="W34" s="2"/>
       <c r="X34" s="2"/>
       <c r="Y34" s="2"/>
-      <c r="Z34" s="51"/>
+      <c r="Z34" s="46"/>
       <c r="AA34" s="1"/>
       <c r="AB34" s="6"/>
     </row>
@@ -2700,14 +2672,14 @@
       <c r="P35" s="5"/>
       <c r="Q35" s="5"/>
       <c r="R35" s="5"/>
-      <c r="S35" s="45"/>
-      <c r="T35" s="45"/>
-      <c r="U35" s="47"/>
+      <c r="S35" s="40"/>
+      <c r="T35" s="40"/>
+      <c r="U35" s="42"/>
       <c r="V35" s="5"/>
       <c r="W35" s="5"/>
-      <c r="X35" s="45"/>
-      <c r="Y35" s="45"/>
-      <c r="Z35" s="54"/>
+      <c r="X35" s="40"/>
+      <c r="Y35" s="40"/>
+      <c r="Z35" s="49"/>
       <c r="AA35" s="4">
         <f>SUM(E35:Z35)</f>
         <v>0</v>
@@ -2744,12 +2716,12 @@
       <c r="R36" s="8"/>
       <c r="S36" s="8"/>
       <c r="T36" s="8"/>
-      <c r="U36" s="49"/>
+      <c r="U36" s="44"/>
       <c r="V36" s="8"/>
       <c r="W36" s="8"/>
       <c r="X36" s="8"/>
       <c r="Y36" s="8"/>
-      <c r="Z36" s="55"/>
+      <c r="Z36" s="50"/>
       <c r="AA36" s="4">
         <f>SUM(E36:Z36)</f>
         <v>0</v>
@@ -2763,10 +2735,10 @@
       <c r="A37" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B37" s="35" t="s">
+      <c r="B37" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="C37" s="35"/>
+      <c r="C37" s="61"/>
       <c r="D37" s="1"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
@@ -2789,7 +2761,7 @@
       <c r="W37" s="2"/>
       <c r="X37" s="2"/>
       <c r="Y37" s="2"/>
-      <c r="Z37" s="51"/>
+      <c r="Z37" s="46"/>
       <c r="AA37" s="1"/>
       <c r="AB37" s="1"/>
     </row>
@@ -2804,28 +2776,28 @@
       <c r="D38" s="4">
         <v>3</v>
       </c>
-      <c r="E38" s="45"/>
-      <c r="F38" s="45"/>
-      <c r="G38" s="45"/>
-      <c r="H38" s="47"/>
-      <c r="I38" s="45"/>
-      <c r="J38" s="45"/>
-      <c r="K38" s="45"/>
-      <c r="L38" s="45"/>
-      <c r="M38" s="45"/>
-      <c r="N38" s="45"/>
-      <c r="O38" s="45"/>
-      <c r="P38" s="45"/>
-      <c r="Q38" s="45"/>
-      <c r="R38" s="45"/>
-      <c r="S38" s="45"/>
-      <c r="T38" s="45"/>
-      <c r="U38" s="47"/>
-      <c r="V38" s="45"/>
-      <c r="W38" s="45"/>
-      <c r="X38" s="45"/>
-      <c r="Y38" s="45"/>
-      <c r="Z38" s="54"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="40"/>
+      <c r="G38" s="40"/>
+      <c r="H38" s="42"/>
+      <c r="I38" s="40"/>
+      <c r="J38" s="40"/>
+      <c r="K38" s="40"/>
+      <c r="L38" s="40"/>
+      <c r="M38" s="40"/>
+      <c r="N38" s="40"/>
+      <c r="O38" s="40"/>
+      <c r="P38" s="40"/>
+      <c r="Q38" s="40"/>
+      <c r="R38" s="40"/>
+      <c r="S38" s="40"/>
+      <c r="T38" s="40"/>
+      <c r="U38" s="42"/>
+      <c r="V38" s="40"/>
+      <c r="W38" s="40"/>
+      <c r="X38" s="40"/>
+      <c r="Y38" s="40"/>
+      <c r="Z38" s="49"/>
       <c r="AA38" s="4">
         <f>SUM(E38:Z38)</f>
         <v>0</v>
@@ -2846,14 +2818,16 @@
       <c r="D39" s="4">
         <v>10</v>
       </c>
-      <c r="E39" s="45">
+      <c r="E39" s="40">
         <v>5</v>
       </c>
-      <c r="F39" s="46">
+      <c r="F39" s="41">
+        <v>6</v>
+      </c>
+      <c r="G39" s="40">
         <v>3</v>
       </c>
-      <c r="G39" s="45"/>
-      <c r="H39" s="47"/>
+      <c r="H39" s="42"/>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
@@ -2871,14 +2845,14 @@
       <c r="W39" s="5"/>
       <c r="X39" s="5"/>
       <c r="Y39" s="5"/>
-      <c r="Z39" s="52"/>
+      <c r="Z39" s="47"/>
       <c r="AA39" s="4">
         <f>SUM(E39:Z39)</f>
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="AB39" s="4">
         <f>D39-AA39</f>
-        <v>2</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.3">
@@ -2892,14 +2866,14 @@
       <c r="D40" s="4">
         <v>2</v>
       </c>
-      <c r="E40" s="45">
+      <c r="E40" s="40">
         <v>0.5</v>
       </c>
-      <c r="F40" s="46">
+      <c r="F40" s="41">
         <v>1</v>
       </c>
-      <c r="G40" s="45"/>
-      <c r="H40" s="47"/>
+      <c r="G40" s="40"/>
+      <c r="H40" s="42"/>
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
@@ -2917,7 +2891,7 @@
       <c r="W40" s="5"/>
       <c r="X40" s="5"/>
       <c r="Y40" s="5"/>
-      <c r="Z40" s="52"/>
+      <c r="Z40" s="47"/>
       <c r="AA40" s="4">
         <f>SUM(E40:Z40)</f>
         <v>1.5</v>
@@ -2938,32 +2912,34 @@
       <c r="D41" s="4">
         <v>22</v>
       </c>
-      <c r="E41" s="45">
+      <c r="E41" s="40">
         <v>1</v>
       </c>
-      <c r="F41" s="46">
+      <c r="F41" s="41">
         <v>2</v>
       </c>
-      <c r="G41" s="45"/>
-      <c r="H41" s="47"/>
-      <c r="I41" s="45"/>
-      <c r="J41" s="45"/>
-      <c r="K41" s="45"/>
-      <c r="L41" s="45"/>
-      <c r="M41" s="45"/>
-      <c r="N41" s="45"/>
-      <c r="O41" s="45"/>
-      <c r="P41" s="45"/>
-      <c r="Q41" s="45"/>
-      <c r="R41" s="45"/>
-      <c r="S41" s="45"/>
-      <c r="T41" s="45"/>
-      <c r="U41" s="47"/>
-      <c r="V41" s="45"/>
-      <c r="W41" s="45"/>
-      <c r="X41" s="45"/>
-      <c r="Y41" s="45"/>
-      <c r="Z41" s="54"/>
+      <c r="G41" s="40">
+        <v>1</v>
+      </c>
+      <c r="H41" s="42"/>
+      <c r="I41" s="40"/>
+      <c r="J41" s="40"/>
+      <c r="K41" s="40"/>
+      <c r="L41" s="40"/>
+      <c r="M41" s="40"/>
+      <c r="N41" s="40"/>
+      <c r="O41" s="40"/>
+      <c r="P41" s="40"/>
+      <c r="Q41" s="40"/>
+      <c r="R41" s="40"/>
+      <c r="S41" s="40"/>
+      <c r="T41" s="40"/>
+      <c r="U41" s="42"/>
+      <c r="V41" s="40"/>
+      <c r="W41" s="40"/>
+      <c r="X41" s="40"/>
+      <c r="Y41" s="40"/>
+      <c r="Z41" s="49"/>
       <c r="AA41" s="4"/>
       <c r="AB41" s="4"/>
     </row>
@@ -2979,46 +2955,48 @@
         <v>5</v>
       </c>
       <c r="E42" s="8"/>
-      <c r="F42" s="48">
+      <c r="F42" s="43">
         <v>0.25</v>
       </c>
-      <c r="G42" s="48"/>
-      <c r="H42" s="49"/>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
-      <c r="K42" s="48"/>
-      <c r="L42" s="48"/>
-      <c r="M42" s="48"/>
-      <c r="N42" s="48"/>
-      <c r="O42" s="48"/>
-      <c r="P42" s="48"/>
-      <c r="Q42" s="48"/>
-      <c r="R42" s="48"/>
-      <c r="S42" s="48"/>
-      <c r="T42" s="48"/>
-      <c r="U42" s="49"/>
-      <c r="V42" s="48"/>
-      <c r="W42" s="48"/>
-      <c r="X42" s="48"/>
-      <c r="Y42" s="48"/>
-      <c r="Z42" s="55"/>
+      <c r="G42" s="43">
+        <v>0.25</v>
+      </c>
+      <c r="H42" s="44"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
+      <c r="K42" s="43"/>
+      <c r="L42" s="43"/>
+      <c r="M42" s="43"/>
+      <c r="N42" s="43"/>
+      <c r="O42" s="43"/>
+      <c r="P42" s="43"/>
+      <c r="Q42" s="43"/>
+      <c r="R42" s="43"/>
+      <c r="S42" s="43"/>
+      <c r="T42" s="43"/>
+      <c r="U42" s="44"/>
+      <c r="V42" s="43"/>
+      <c r="W42" s="43"/>
+      <c r="X42" s="43"/>
+      <c r="Y42" s="43"/>
+      <c r="Z42" s="50"/>
       <c r="AA42" s="7">
         <f>SUM(E42:Z42)</f>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="AB42" s="7">
         <f>D42-AA42</f>
-        <v>4.75</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="43" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B43" s="35" t="s">
+      <c r="B43" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="C43" s="35"/>
+      <c r="C43" s="61"/>
       <c r="D43" s="1">
         <v>42</v>
       </c>
@@ -3043,7 +3021,7 @@
       <c r="W43" s="2"/>
       <c r="X43" s="2"/>
       <c r="Y43" s="2"/>
-      <c r="Z43" s="51"/>
+      <c r="Z43" s="46"/>
       <c r="AA43" s="10">
         <f>SUM(E43:Z43)</f>
         <v>0</v>
@@ -3079,121 +3057,121 @@
       <c r="W44" s="2"/>
       <c r="X44" s="2"/>
       <c r="Y44" s="2"/>
-      <c r="Z44" s="51"/>
+      <c r="Z44" s="46"/>
       <c r="AA44" s="8"/>
       <c r="AB44" s="8"/>
     </row>
     <row r="45" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="39" t="s">
+      <c r="A45" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="B45" s="40"/>
-      <c r="C45" s="40"/>
+      <c r="B45" s="59"/>
+      <c r="C45" s="59"/>
       <c r="D45" s="10">
         <f>SUM(D2:D44)</f>
         <v>549</v>
       </c>
       <c r="E45" s="9">
-        <f>SUM(E2:E43)</f>
+        <f t="shared" ref="E45:Z45" si="2">SUM(E2:E43)</f>
         <v>8</v>
       </c>
       <c r="F45" s="9">
-        <f>SUM(F2:F43)</f>
-        <v>6.25</v>
+        <f t="shared" si="2"/>
+        <v>14.25</v>
       </c>
       <c r="G45" s="9">
-        <f>SUM(G2:G43)</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>4.25</v>
       </c>
       <c r="H45" s="32">
-        <f>SUM(H2:H43)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I45" s="9">
-        <f>SUM(I2:I43)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J45" s="9">
-        <f>SUM(J2:J43)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K45" s="9">
-        <f>SUM(K2:K43)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L45" s="9">
-        <f>SUM(L2:L43)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M45" s="9">
-        <f>SUM(M2:M43)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N45" s="9">
-        <f>SUM(N2:N43)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O45" s="9">
-        <f>SUM(O2:O43)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P45" s="9">
-        <f>SUM(P2:P43)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q45" s="9">
-        <f>SUM(Q2:Q43)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R45" s="9">
-        <f>SUM(R2:R43)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S45" s="9">
-        <f>SUM(S2:S43)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T45" s="9">
-        <f>SUM(T2:T43)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U45" s="27">
-        <f>SUM(U2:U43)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="V45" s="9">
-        <f>SUM(V2:V43)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="W45" s="9">
-        <f>SUM(W2:W43)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X45" s="9">
-        <f>SUM(X2:X43)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Y45" s="9">
-        <f>SUM(Y2:Y43)</f>
-        <v>0</v>
-      </c>
-      <c r="Z45" s="57">
-        <f>SUM(Z2:Z43)</f>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z45" s="52">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AA45" s="7">
         <f>SUM(E45:Z45)</f>
-        <v>14.25</v>
+        <v>26.5</v>
       </c>
       <c r="AB45" s="7">
         <f>D45-AA45</f>
-        <v>534.75</v>
+        <v>522.5</v>
       </c>
     </row>
     <row r="46" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="38"/>
-      <c r="B46" s="38"/>
-      <c r="C46" s="38"/>
+      <c r="A46" s="36"/>
+      <c r="B46" s="36"/>
+      <c r="C46" s="36"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
@@ -3221,98 +3199,98 @@
       <c r="AB46" s="5"/>
     </row>
     <row r="47" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="39" t="s">
+      <c r="A47" s="58" t="s">
         <v>102</v>
       </c>
-      <c r="B47" s="40"/>
-      <c r="C47" s="40"/>
-      <c r="D47" s="43"/>
-      <c r="E47" s="41">
+      <c r="B47" s="59"/>
+      <c r="C47" s="59"/>
+      <c r="D47" s="60"/>
+      <c r="E47" s="37">
         <f>($D$45 -12*16-6*40)/(16+6) + 12</f>
         <v>17.31818181818182</v>
       </c>
-      <c r="F47" s="41">
-        <f t="shared" ref="F47:T47" si="0">($D$45 -12*16-6*40)/(16+6) + 12</f>
+      <c r="F47" s="37">
+        <f t="shared" ref="F47:T47" si="3">($D$45 -12*16-6*40)/(16+6) + 12</f>
         <v>17.31818181818182</v>
       </c>
-      <c r="G47" s="41">
-        <f t="shared" si="0"/>
+      <c r="G47" s="37">
+        <f t="shared" si="3"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="H47" s="41">
-        <f t="shared" si="0"/>
+      <c r="H47" s="37">
+        <f t="shared" si="3"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="I47" s="41">
-        <f t="shared" si="0"/>
+      <c r="I47" s="37">
+        <f t="shared" si="3"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="J47" s="41">
-        <f t="shared" si="0"/>
+      <c r="J47" s="37">
+        <f t="shared" si="3"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="K47" s="41">
-        <f t="shared" si="0"/>
+      <c r="K47" s="37">
+        <f t="shared" si="3"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="L47" s="41">
-        <f t="shared" si="0"/>
+      <c r="L47" s="37">
+        <f t="shared" si="3"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="M47" s="41">
-        <f t="shared" si="0"/>
+      <c r="M47" s="37">
+        <f t="shared" si="3"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="N47" s="41">
-        <f t="shared" si="0"/>
+      <c r="N47" s="37">
+        <f t="shared" si="3"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="O47" s="41">
-        <f t="shared" si="0"/>
+      <c r="O47" s="37">
+        <f t="shared" si="3"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="P47" s="41">
-        <f t="shared" si="0"/>
+      <c r="P47" s="37">
+        <f t="shared" si="3"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="Q47" s="41">
-        <f t="shared" si="0"/>
+      <c r="Q47" s="37">
+        <f t="shared" si="3"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="R47" s="41">
-        <f t="shared" si="0"/>
+      <c r="R47" s="37">
+        <f t="shared" si="3"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="S47" s="41">
-        <f t="shared" si="0"/>
+      <c r="S47" s="37">
+        <f t="shared" si="3"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="T47" s="41">
-        <f t="shared" si="0"/>
+      <c r="T47" s="37">
+        <f t="shared" si="3"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="U47" s="41">
+      <c r="U47" s="37">
         <f>($D$45 -12*16-6*40)/(16+6) + 40</f>
         <v>45.31818181818182</v>
       </c>
-      <c r="V47" s="41">
-        <f t="shared" ref="V47:Z47" si="1">($D$45 -12*16-6*40)/(16+6) + 40</f>
+      <c r="V47" s="37">
+        <f t="shared" ref="V47:Z47" si="4">($D$45 -12*16-6*40)/(16+6) + 40</f>
         <v>45.31818181818182</v>
       </c>
-      <c r="W47" s="41">
-        <f t="shared" si="1"/>
+      <c r="W47" s="37">
+        <f t="shared" si="4"/>
         <v>45.31818181818182</v>
       </c>
-      <c r="X47" s="41">
-        <f t="shared" si="1"/>
+      <c r="X47" s="37">
+        <f t="shared" si="4"/>
         <v>45.31818181818182</v>
       </c>
-      <c r="Y47" s="41">
-        <f t="shared" si="1"/>
+      <c r="Y47" s="37">
+        <f t="shared" si="4"/>
         <v>45.31818181818182</v>
       </c>
-      <c r="Z47" s="42">
-        <f t="shared" si="1"/>
+      <c r="Z47" s="38">
+        <f t="shared" si="4"/>
         <v>45.31818181818182</v>
       </c>
       <c r="AA47" s="13">
@@ -3321,103 +3299,109 @@
       </c>
     </row>
     <row r="48" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="39" t="s">
+      <c r="A48" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="B48" s="40"/>
-      <c r="C48" s="40"/>
-      <c r="D48" s="43"/>
-      <c r="E48" s="41">
-        <f>E47-E45</f>
+      <c r="B48" s="59"/>
+      <c r="C48" s="59"/>
+      <c r="D48" s="60"/>
+      <c r="E48" s="37">
+        <f t="shared" ref="E48:Z48" si="5">E47-E45</f>
         <v>9.3181818181818201</v>
       </c>
-      <c r="F48" s="41">
-        <f>F47-F45</f>
-        <v>11.06818181818182</v>
-      </c>
-      <c r="G48" s="41">
-        <f>G47-G45</f>
+      <c r="F48" s="37">
+        <f t="shared" si="5"/>
+        <v>3.0681818181818201</v>
+      </c>
+      <c r="G48" s="37">
+        <f t="shared" si="5"/>
+        <v>13.06818181818182</v>
+      </c>
+      <c r="H48" s="37">
+        <f t="shared" si="5"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="H48" s="41">
-        <f>H47-H45</f>
+      <c r="I48" s="37">
+        <f t="shared" si="5"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="I48" s="41">
-        <f>I47-I45</f>
+      <c r="J48" s="37">
+        <f t="shared" si="5"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="J48" s="41">
-        <f>J47-J45</f>
+      <c r="K48" s="37">
+        <f t="shared" si="5"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="K48" s="41">
-        <f>K47-K45</f>
+      <c r="L48" s="37">
+        <f t="shared" si="5"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="L48" s="41">
-        <f>L47-L45</f>
+      <c r="M48" s="37">
+        <f t="shared" si="5"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="M48" s="41">
-        <f>M47-M45</f>
+      <c r="N48" s="37">
+        <f t="shared" si="5"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="N48" s="41">
-        <f>N47-N45</f>
+      <c r="O48" s="37">
+        <f t="shared" si="5"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="O48" s="41">
-        <f>O47-O45</f>
+      <c r="P48" s="37">
+        <f t="shared" si="5"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="P48" s="41">
-        <f>P47-P45</f>
+      <c r="Q48" s="37">
+        <f t="shared" si="5"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="Q48" s="41">
-        <f>Q47-Q45</f>
+      <c r="R48" s="37">
+        <f t="shared" si="5"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="R48" s="41">
-        <f>R47-R45</f>
+      <c r="S48" s="37">
+        <f t="shared" si="5"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="S48" s="41">
-        <f>S47-S45</f>
+      <c r="T48" s="37">
+        <f t="shared" si="5"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="T48" s="41">
-        <f>T47-T45</f>
-        <v>17.31818181818182</v>
-      </c>
-      <c r="U48" s="41">
-        <f>U47-U45</f>
+      <c r="U48" s="37">
+        <f t="shared" si="5"/>
         <v>45.31818181818182</v>
       </c>
-      <c r="V48" s="41">
-        <f>V47-V45</f>
+      <c r="V48" s="37">
+        <f t="shared" si="5"/>
         <v>45.31818181818182</v>
       </c>
-      <c r="W48" s="41">
-        <f>W47-W45</f>
+      <c r="W48" s="37">
+        <f t="shared" si="5"/>
         <v>45.31818181818182</v>
       </c>
-      <c r="X48" s="41">
-        <f>X47-X45</f>
+      <c r="X48" s="37">
+        <f t="shared" si="5"/>
         <v>45.31818181818182</v>
       </c>
-      <c r="Y48" s="41">
-        <f>Y47-Y45</f>
+      <c r="Y48" s="37">
+        <f t="shared" si="5"/>
         <v>45.31818181818182</v>
       </c>
-      <c r="Z48" s="42">
-        <f>Z47-Z45</f>
+      <c r="Z48" s="38">
+        <f t="shared" si="5"/>
         <v>45.31818181818182</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="A47:D47"/>
     <mergeCell ref="A48:D48"/>
     <mergeCell ref="B31:C31"/>
@@ -3425,12 +3409,6 @@
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="A45:C45"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B17:C17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="AB2:AB46">

</xml_diff>

<commit_message>
update spec & planif
</commit_message>
<xml_diff>
--- a/Documentation/Planification.xlsx
+++ b/Documentation/Planification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/371c2caacf93074d/Documents/HEIG/TB Driver Brushless/TB-Driver-Brushless/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="710" documentId="8_{CB7147DC-5DFD-4F3C-85F9-1BD4040EC95A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{82A87D74-27E8-490A-8B4D-EFF7500EBD41}"/>
+  <xr:revisionPtr revIDLastSave="734" documentId="8_{CB7147DC-5DFD-4F3C-85F9-1BD4040EC95A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1CDA0BF8-1D8C-4394-BA8A-C5FD8EB216F3}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E4DCEC7E-A84B-4A69-AC68-472FA9C158BB}"/>
   </bookViews>
@@ -732,7 +732,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -905,20 +905,32 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1267,8 +1279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09FBCC03-12B2-4877-A171-7A10D6B76BA3}">
   <dimension ref="A1:AB48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="58" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="58" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AH37" sqref="AH37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1289,10 +1301,10 @@
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="59"/>
+      <c r="C1" s="62"/>
       <c r="D1" s="14" t="s">
         <v>35</v>
       </c>
@@ -1373,10 +1385,10 @@
       <c r="A2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="58"/>
+      <c r="C2" s="61"/>
       <c r="D2" s="1"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -1583,10 +1595,10 @@
       <c r="A7" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="58" t="s">
+      <c r="B7" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="58"/>
+      <c r="C7" s="61"/>
       <c r="D7" s="1"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -1735,10 +1747,10 @@
       <c r="A11" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="58" t="s">
+      <c r="B11" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="58"/>
+      <c r="C11" s="61"/>
       <c r="D11" s="1"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -1762,14 +1774,8 @@
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
       <c r="Z11" s="46"/>
-      <c r="AA11" s="1">
-        <f>SUM(E11:Z11)</f>
-        <v>0</v>
-      </c>
-      <c r="AB11" s="6">
-        <f>D11-AA11</f>
-        <v>0</v>
-      </c>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="6"/>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" s="34"/>
@@ -1802,8 +1808,14 @@
       <c r="X12" s="5"/>
       <c r="Y12" s="5"/>
       <c r="Z12" s="47"/>
-      <c r="AA12" s="4"/>
-      <c r="AB12" s="6"/>
+      <c r="AA12" s="4">
+        <f t="shared" ref="AA12:AA15" si="0">SUM(E12:Z12)</f>
+        <v>13</v>
+      </c>
+      <c r="AB12" s="6">
+        <f t="shared" ref="AB12:AB16" si="1">D12-AA12</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" s="34"/>
@@ -1834,8 +1846,14 @@
       <c r="X13" s="5"/>
       <c r="Y13" s="5"/>
       <c r="Z13" s="47"/>
-      <c r="AA13" s="4"/>
-      <c r="AB13" s="6"/>
+      <c r="AA13" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB13" s="6">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" s="34"/>
@@ -1866,8 +1884,14 @@
       <c r="X14" s="5"/>
       <c r="Y14" s="5"/>
       <c r="Z14" s="47"/>
-      <c r="AA14" s="4"/>
-      <c r="AB14" s="6"/>
+      <c r="AA14" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB14" s="6">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" s="34"/>
@@ -1898,8 +1922,14 @@
       <c r="X15" s="5"/>
       <c r="Y15" s="5"/>
       <c r="Z15" s="47"/>
-      <c r="AA15" s="4"/>
-      <c r="AB15" s="6"/>
+      <c r="AA15" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB15" s="6">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="20"/>
@@ -1930,12 +1960,12 @@
       <c r="X16" s="8"/>
       <c r="Y16" s="8"/>
       <c r="Z16" s="48"/>
-      <c r="AA16" s="4">
+      <c r="AA16" s="7">
         <f>SUM(E16:Z16)</f>
         <v>0</v>
       </c>
       <c r="AB16" s="6">
-        <f>D16-AA16</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
@@ -1943,10 +1973,10 @@
       <c r="A17" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="58" t="s">
+      <c r="B17" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="58"/>
+      <c r="C17" s="61"/>
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -1970,7 +2000,7 @@
       <c r="X17" s="2"/>
       <c r="Y17" s="2"/>
       <c r="Z17" s="46"/>
-      <c r="AA17" s="1"/>
+      <c r="AA17" s="4"/>
       <c r="AB17" s="1"/>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.3">
@@ -2109,10 +2139,10 @@
       <c r="A21" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="58" t="s">
+      <c r="B21" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="58"/>
+      <c r="C21" s="61"/>
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -2173,11 +2203,11 @@
       <c r="Y22" s="5"/>
       <c r="Z22" s="47"/>
       <c r="AA22" s="4">
-        <f t="shared" ref="AA22:AA31" si="0">SUM(E22:Z22)</f>
+        <f t="shared" ref="AA22:AA34" si="2">SUM(E22:Z22)</f>
         <v>0</v>
       </c>
       <c r="AB22" s="6">
-        <f t="shared" ref="AB22:AB31" si="1">D22-AA22</f>
+        <f t="shared" ref="AB22:AB36" si="3">D22-AA22</f>
         <v>20</v>
       </c>
     </row>
@@ -2215,11 +2245,11 @@
       <c r="Y23" s="5"/>
       <c r="Z23" s="47"/>
       <c r="AA23" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB23" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
     </row>
@@ -2257,11 +2287,11 @@
       <c r="Y24" s="5"/>
       <c r="Z24" s="47"/>
       <c r="AA24" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB24" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
     </row>
@@ -2299,11 +2329,11 @@
       <c r="Y25" s="5"/>
       <c r="Z25" s="47"/>
       <c r="AA25" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB25" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
     </row>
@@ -2341,11 +2371,11 @@
       <c r="Y26" s="5"/>
       <c r="Z26" s="47"/>
       <c r="AA26" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB26" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
     </row>
@@ -2383,11 +2413,11 @@
       <c r="Y27" s="5"/>
       <c r="Z27" s="47"/>
       <c r="AA27" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB27" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
     </row>
@@ -2425,11 +2455,11 @@
       <c r="Y28" s="5"/>
       <c r="Z28" s="47"/>
       <c r="AA28" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB28" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
     </row>
@@ -2467,11 +2497,11 @@
       <c r="Y29" s="5"/>
       <c r="Z29" s="47"/>
       <c r="AA29" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB29" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
     </row>
@@ -2509,11 +2539,11 @@
       <c r="Y30" s="43"/>
       <c r="Z30" s="50"/>
       <c r="AA30" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB30" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
     </row>
@@ -2521,10 +2551,10 @@
       <c r="A31" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="58" t="s">
+      <c r="B31" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="58"/>
+      <c r="C31" s="61"/>
       <c r="D31" s="1"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
@@ -2548,14 +2578,8 @@
       <c r="X31" s="2"/>
       <c r="Y31" s="2"/>
       <c r="Z31" s="46"/>
-      <c r="AA31" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AB31" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="AA31" s="63"/>
+      <c r="AB31" s="1"/>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A32" s="34"/>
@@ -2588,8 +2612,14 @@
       <c r="X32" s="5"/>
       <c r="Y32" s="40"/>
       <c r="Z32" s="49"/>
-      <c r="AA32" s="4"/>
-      <c r="AB32" s="4"/>
+      <c r="AA32" s="64">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AB32" s="4">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
     </row>
     <row r="33" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="34"/>
@@ -2622,17 +2652,23 @@
       <c r="X33" s="5"/>
       <c r="Y33" s="40"/>
       <c r="Z33" s="49"/>
-      <c r="AA33" s="4"/>
-      <c r="AB33" s="4"/>
+      <c r="AA33" s="64">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AB33" s="4">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A34" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="58" t="s">
+      <c r="B34" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="58"/>
+      <c r="C34" s="61"/>
       <c r="D34" s="1"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
@@ -2656,8 +2692,8 @@
       <c r="X34" s="2"/>
       <c r="Y34" s="2"/>
       <c r="Z34" s="46"/>
-      <c r="AA34" s="1"/>
-      <c r="AB34" s="6"/>
+      <c r="AA34" s="63"/>
+      <c r="AB34" s="1"/>
     </row>
     <row r="35" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A35" s="18" t="s">
@@ -2692,12 +2728,12 @@
       <c r="X35" s="40"/>
       <c r="Y35" s="40"/>
       <c r="Z35" s="49"/>
-      <c r="AA35" s="4">
+      <c r="AA35" s="64">
         <f>SUM(E35:Z35)</f>
         <v>0</v>
       </c>
-      <c r="AB35" s="6">
-        <f>D35-AA35</f>
+      <c r="AB35" s="4">
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
     </row>
@@ -2734,12 +2770,12 @@
       <c r="X36" s="8"/>
       <c r="Y36" s="8"/>
       <c r="Z36" s="50"/>
-      <c r="AA36" s="4">
+      <c r="AA36" s="65">
         <f>SUM(E36:Z36)</f>
         <v>0</v>
       </c>
-      <c r="AB36" s="6">
-        <f>D36-AA36</f>
+      <c r="AB36" s="7">
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
     </row>
@@ -2747,10 +2783,10 @@
       <c r="A37" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B37" s="58" t="s">
+      <c r="B37" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="C37" s="58"/>
+      <c r="C37" s="61"/>
       <c r="D37" s="1"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
@@ -2774,8 +2810,8 @@
       <c r="X37" s="2"/>
       <c r="Y37" s="2"/>
       <c r="Z37" s="46"/>
-      <c r="AA37" s="1"/>
-      <c r="AB37" s="1"/>
+      <c r="AA37" s="4"/>
+      <c r="AB37" s="4"/>
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A38" s="18" t="s">
@@ -2840,7 +2876,9 @@
         <v>3</v>
       </c>
       <c r="H39" s="42"/>
-      <c r="I39" s="5"/>
+      <c r="I39" s="5">
+        <v>0.5</v>
+      </c>
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
@@ -2860,11 +2898,11 @@
       <c r="Z39" s="47"/>
       <c r="AA39" s="4">
         <f>SUM(E39:Z39)</f>
-        <v>14</v>
+        <v>14.5</v>
       </c>
       <c r="AB39" s="4">
         <f>D39-AA39</f>
-        <v>-4</v>
+        <v>-4.5</v>
       </c>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.3">
@@ -2936,7 +2974,9 @@
       <c r="H41" s="42">
         <v>1</v>
       </c>
-      <c r="I41" s="40"/>
+      <c r="I41" s="40">
+        <v>1</v>
+      </c>
       <c r="J41" s="40"/>
       <c r="K41" s="40"/>
       <c r="L41" s="40"/>
@@ -2954,8 +2994,14 @@
       <c r="X41" s="40"/>
       <c r="Y41" s="40"/>
       <c r="Z41" s="49"/>
-      <c r="AA41" s="4"/>
-      <c r="AB41" s="4"/>
+      <c r="AA41" s="4">
+        <f>SUM(E41:Z41)</f>
+        <v>6</v>
+      </c>
+      <c r="AB41" s="4">
+        <f>D41-AA41</f>
+        <v>16</v>
+      </c>
     </row>
     <row r="42" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="20" t="s">
@@ -2978,7 +3024,9 @@
       <c r="H42" s="44">
         <v>0.25</v>
       </c>
-      <c r="I42" s="43"/>
+      <c r="I42" s="43">
+        <v>0.25</v>
+      </c>
       <c r="J42" s="43"/>
       <c r="K42" s="43"/>
       <c r="L42" s="43"/>
@@ -2998,21 +3046,21 @@
       <c r="Z42" s="50"/>
       <c r="AA42" s="7">
         <f>SUM(E42:Z42)</f>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="AB42" s="7">
         <f>D42-AA42</f>
-        <v>4.25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B43" s="58" t="s">
+      <c r="B43" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="C43" s="58"/>
+      <c r="C43" s="61"/>
       <c r="D43" s="1">
         <v>42</v>
       </c>
@@ -3078,110 +3126,110 @@
       <c r="AB44" s="8"/>
     </row>
     <row r="45" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="60" t="s">
+      <c r="A45" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="B45" s="61"/>
-      <c r="C45" s="61"/>
+      <c r="B45" s="59"/>
+      <c r="C45" s="59"/>
       <c r="D45" s="10">
         <f>SUM(D2:D44)</f>
         <v>549</v>
       </c>
       <c r="E45" s="9">
-        <f t="shared" ref="E45:Z45" si="2">SUM(E2:E43)</f>
+        <f t="shared" ref="E45:Z45" si="4">SUM(E2:E43)</f>
         <v>8</v>
       </c>
       <c r="F45" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>14.25</v>
       </c>
       <c r="G45" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>16.25</v>
       </c>
       <c r="H45" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>18.25</v>
       </c>
       <c r="I45" s="9">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>1.75</v>
       </c>
       <c r="J45" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K45" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L45" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M45" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N45" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O45" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P45" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q45" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="R45" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S45" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T45" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U45" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="V45" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="W45" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="X45" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Y45" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Z45" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AA45" s="7">
         <f>SUM(E45:Z45)</f>
-        <v>56.75</v>
+        <v>58.5</v>
       </c>
       <c r="AB45" s="7">
         <f>D45-AA45</f>
-        <v>492.25</v>
+        <v>490.5</v>
       </c>
     </row>
     <row r="46" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -3215,74 +3263,74 @@
       <c r="AB46" s="5"/>
     </row>
     <row r="47" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="60" t="s">
+      <c r="A47" s="58" t="s">
         <v>102</v>
       </c>
-      <c r="B47" s="61"/>
-      <c r="C47" s="61"/>
-      <c r="D47" s="62"/>
+      <c r="B47" s="59"/>
+      <c r="C47" s="59"/>
+      <c r="D47" s="60"/>
       <c r="E47" s="37">
         <f>($D$45 -12*16-6*40)/(16+6) + 12</f>
         <v>17.31818181818182</v>
       </c>
       <c r="F47" s="37">
-        <f t="shared" ref="F47:T47" si="3">($D$45 -12*16-6*40)/(16+6) + 12</f>
+        <f t="shared" ref="F47:T47" si="5">($D$45 -12*16-6*40)/(16+6) + 12</f>
         <v>17.31818181818182</v>
       </c>
       <c r="G47" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17.31818181818182</v>
       </c>
       <c r="H47" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17.31818181818182</v>
       </c>
       <c r="I47" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17.31818181818182</v>
       </c>
       <c r="J47" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17.31818181818182</v>
       </c>
       <c r="K47" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17.31818181818182</v>
       </c>
       <c r="L47" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17.31818181818182</v>
       </c>
       <c r="M47" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17.31818181818182</v>
       </c>
       <c r="N47" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17.31818181818182</v>
       </c>
       <c r="O47" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17.31818181818182</v>
       </c>
       <c r="P47" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17.31818181818182</v>
       </c>
       <c r="Q47" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17.31818181818182</v>
       </c>
       <c r="R47" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17.31818181818182</v>
       </c>
       <c r="S47" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17.31818181818182</v>
       </c>
       <c r="T47" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17.31818181818182</v>
       </c>
       <c r="U47" s="37">
@@ -3290,128 +3338,134 @@
         <v>45.31818181818182</v>
       </c>
       <c r="V47" s="37">
-        <f t="shared" ref="V47:Z47" si="4">($D$45 -12*16-6*40)/(16+6) + 40</f>
+        <f t="shared" ref="V47:Z47" si="6">($D$45 -12*16-6*40)/(16+6) + 40</f>
         <v>45.31818181818182</v>
       </c>
       <c r="W47" s="37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>45.31818181818182</v>
       </c>
       <c r="X47" s="37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>45.31818181818182</v>
       </c>
       <c r="Y47" s="37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>45.31818181818182</v>
       </c>
       <c r="Z47" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>45.31818181818182</v>
       </c>
-      <c r="AA47" s="13">
+      <c r="AA47" s="66">
         <f>SUM(E47:Z47)</f>
         <v>549</v>
       </c>
     </row>
     <row r="48" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="60" t="s">
+      <c r="A48" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="B48" s="61"/>
-      <c r="C48" s="61"/>
-      <c r="D48" s="62"/>
+      <c r="B48" s="59"/>
+      <c r="C48" s="59"/>
+      <c r="D48" s="60"/>
       <c r="E48" s="37">
-        <f t="shared" ref="E48:Z48" si="5">E47-E45</f>
+        <f t="shared" ref="E48:Z48" si="7">E47-E45</f>
         <v>9.3181818181818201</v>
       </c>
       <c r="F48" s="37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.0681818181818201</v>
       </c>
       <c r="G48" s="37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.0681818181818201</v>
       </c>
       <c r="H48" s="37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-0.93181818181817988</v>
       </c>
       <c r="I48" s="37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
+        <v>15.56818181818182</v>
+      </c>
+      <c r="J48" s="37">
+        <f t="shared" si="7"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="J48" s="37">
-        <f t="shared" si="5"/>
+      <c r="K48" s="37">
+        <f t="shared" si="7"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="K48" s="37">
-        <f t="shared" si="5"/>
+      <c r="L48" s="37">
+        <f t="shared" si="7"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="L48" s="37">
-        <f t="shared" si="5"/>
+      <c r="M48" s="37">
+        <f t="shared" si="7"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="M48" s="37">
-        <f t="shared" si="5"/>
+      <c r="N48" s="37">
+        <f t="shared" si="7"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="N48" s="37">
-        <f t="shared" si="5"/>
+      <c r="O48" s="37">
+        <f t="shared" si="7"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="O48" s="37">
-        <f t="shared" si="5"/>
+      <c r="P48" s="37">
+        <f t="shared" si="7"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="P48" s="37">
-        <f t="shared" si="5"/>
+      <c r="Q48" s="37">
+        <f t="shared" si="7"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="Q48" s="37">
-        <f t="shared" si="5"/>
+      <c r="R48" s="37">
+        <f t="shared" si="7"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="R48" s="37">
-        <f t="shared" si="5"/>
+      <c r="S48" s="37">
+        <f t="shared" si="7"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="S48" s="37">
-        <f t="shared" si="5"/>
+      <c r="T48" s="37">
+        <f t="shared" si="7"/>
         <v>17.31818181818182</v>
       </c>
-      <c r="T48" s="37">
-        <f t="shared" si="5"/>
-        <v>17.31818181818182</v>
-      </c>
       <c r="U48" s="37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>45.31818181818182</v>
       </c>
       <c r="V48" s="37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>45.31818181818182</v>
       </c>
       <c r="W48" s="37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>45.31818181818182</v>
       </c>
       <c r="X48" s="37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>45.31818181818182</v>
       </c>
       <c r="Y48" s="37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>45.31818181818182</v>
       </c>
       <c r="Z48" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>45.31818181818182</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="A47:D47"/>
     <mergeCell ref="A48:D48"/>
     <mergeCell ref="B31:C31"/>
@@ -3419,12 +3473,6 @@
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="A45:C45"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B17:C17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="AB2:AB46">

</xml_diff>

<commit_message>
Update planif + Prj. Status
</commit_message>
<xml_diff>
--- a/Documentation/Planification.xlsx
+++ b/Documentation/Planification.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/371c2caacf93074d/Documents/HEIG/TB Driver Brushless/TB-Driver-Brushless/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="838" documentId="8_{CB7147DC-5DFD-4F3C-85F9-1BD4040EC95A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5B823CF9-5CE0-463A-9A9F-4DBF3FDCF897}"/>
+  <xr:revisionPtr revIDLastSave="1205" documentId="8_{CB7147DC-5DFD-4F3C-85F9-1BD4040EC95A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CFEA6F2-C71B-4A85-8A69-7719CA1C840B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E4DCEC7E-A84B-4A69-AC68-472FA9C158BB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E4DCEC7E-A84B-4A69-AC68-472FA9C158BB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planif. Origine" sheetId="1" r:id="rId1"/>
+    <sheet name="Planif. new" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="126">
   <si>
     <t>N°</t>
   </si>
@@ -340,6 +341,78 @@
   </si>
   <si>
     <t>Schéma d'interface</t>
+  </si>
+  <si>
+    <t>Montage &amp; Contrôle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Placement des composants </t>
+  </si>
+  <si>
+    <t>Nettoyage des cartes</t>
+  </si>
+  <si>
+    <t>Contrôle alims</t>
+  </si>
+  <si>
+    <t>Contrôle pont triphasé</t>
+  </si>
+  <si>
+    <t>Contrôle mesures analogiques</t>
+  </si>
+  <si>
+    <t>T50.30</t>
+  </si>
+  <si>
+    <t>T50.50</t>
+  </si>
+  <si>
+    <t>Test PWM</t>
+  </si>
+  <si>
+    <t>Dead band</t>
+  </si>
+  <si>
+    <t>Séquence PWM (gestion du pont triphasé)</t>
+  </si>
+  <si>
+    <t>T60.10</t>
+  </si>
+  <si>
+    <t>T60.20</t>
+  </si>
+  <si>
+    <t>T60.30</t>
+  </si>
+  <si>
+    <t>T60.40</t>
+  </si>
+  <si>
+    <t>T60.50</t>
+  </si>
+  <si>
+    <t>T60.60</t>
+  </si>
+  <si>
+    <t>T60.70</t>
+  </si>
+  <si>
+    <t>Mesure de tension</t>
+  </si>
+  <si>
+    <t>Mesure de courant</t>
+  </si>
+  <si>
+    <t>Calculs vectoriels</t>
+  </si>
+  <si>
+    <t>Régulation de courant</t>
+  </si>
+  <si>
+    <t>Présentation intérmédiare</t>
+  </si>
+  <si>
+    <t>T100</t>
   </si>
 </sst>
 </file>
@@ -384,7 +457,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -397,8 +470,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="27">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -716,12 +795,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="5" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thick">
+        <color theme="5" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thick">
+        <color theme="5" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -897,6 +1000,72 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -906,10 +1075,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -917,7 +1086,37 @@
     <cellStyle name="Milliers" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1258,10 +1457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09FBCC03-12B2-4877-A171-7A10D6B76BA3}">
-  <dimension ref="A1:Z49"/>
+  <dimension ref="A1:Z53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AF37" sqref="AF37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1280,10 +1479,10 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="63"/>
+      <c r="C1" s="80"/>
       <c r="D1" s="1" t="s">
         <v>35</v>
       </c>
@@ -1358,10 +1557,10 @@
       <c r="A2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="62"/>
+      <c r="C2" s="79"/>
       <c r="D2" s="11"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
@@ -1560,10 +1759,10 @@
       <c r="A7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="62" t="s">
+      <c r="B7" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="62"/>
+      <c r="C7" s="79"/>
       <c r="D7" s="11"/>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
@@ -1718,7 +1917,9 @@
         <v>5</v>
       </c>
       <c r="Q10" s="31"/>
-      <c r="R10" s="31"/>
+      <c r="R10" s="31">
+        <v>1</v>
+      </c>
       <c r="S10" s="32"/>
       <c r="T10" s="31"/>
       <c r="U10" s="31"/>
@@ -1727,21 +1928,21 @@
       <c r="X10" s="33"/>
       <c r="Y10" s="20">
         <f>SUM(E10:X10)</f>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Z10" s="27">
         <f>D10-Y10</f>
-        <v>-16</v>
+        <v>-17</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="62" t="s">
+      <c r="B11" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="62"/>
+      <c r="C11" s="79"/>
       <c r="D11" s="11"/>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
@@ -1793,7 +1994,9 @@
       <c r="N12" s="14"/>
       <c r="O12" s="14"/>
       <c r="Q12" s="14"/>
-      <c r="R12" s="14"/>
+      <c r="R12" s="14">
+        <v>1</v>
+      </c>
       <c r="S12" s="15"/>
       <c r="T12" s="14"/>
       <c r="U12" s="14"/>
@@ -1802,11 +2005,11 @@
       <c r="X12" s="23"/>
       <c r="Y12" s="20">
         <f>SUM(E12:X12)</f>
-        <v>26.5</v>
+        <v>27.5</v>
       </c>
       <c r="Z12" s="24">
         <f>D12-Y12</f>
-        <v>-11.5</v>
+        <v>-12.5</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.3">
@@ -1834,7 +2037,9 @@
       </c>
       <c r="O13" s="14"/>
       <c r="Q13" s="14"/>
-      <c r="R13" s="14"/>
+      <c r="R13" s="14">
+        <v>5</v>
+      </c>
       <c r="S13" s="15"/>
       <c r="T13" s="14"/>
       <c r="U13" s="14"/>
@@ -1843,11 +2048,11 @@
       <c r="X13" s="23"/>
       <c r="Y13" s="20">
         <f>SUM(E13:X13)</f>
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="Z13" s="24">
         <f>D13-Y13</f>
-        <v>-20</v>
+        <v>-25</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.3">
@@ -1870,8 +2075,12 @@
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14"/>
+      <c r="Q14" s="14">
+        <v>15</v>
+      </c>
+      <c r="R14" s="14">
+        <v>18</v>
+      </c>
       <c r="S14" s="15"/>
       <c r="T14" s="14"/>
       <c r="U14" s="14"/>
@@ -1880,11 +2089,11 @@
       <c r="X14" s="23"/>
       <c r="Y14" s="20">
         <f>SUM(E14:X14)</f>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="Z14" s="24">
         <f>D14-Y14</f>
-        <v>40</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
@@ -1966,10 +2175,10 @@
       <c r="A17" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="62" t="s">
+      <c r="B17" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="62"/>
+      <c r="C17" s="79"/>
       <c r="D17" s="11"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
@@ -2019,7 +2228,9 @@
       <c r="P18" s="3">
         <v>6</v>
       </c>
-      <c r="Q18" s="14"/>
+      <c r="Q18" s="14">
+        <v>5</v>
+      </c>
       <c r="R18" s="14"/>
       <c r="S18" s="15"/>
       <c r="T18" s="14"/>
@@ -2029,11 +2240,11 @@
       <c r="X18" s="23"/>
       <c r="Y18" s="20">
         <f>SUM(E18:X18)</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="Z18" s="20">
         <f>D18-Y18</f>
-        <v>-3</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.3">
@@ -2126,10 +2337,10 @@
       <c r="A21" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="62" t="s">
+      <c r="B21" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="62"/>
+      <c r="C21" s="79"/>
       <c r="D21" s="11"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
@@ -2518,10 +2729,10 @@
       <c r="A31" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="62" t="s">
+      <c r="B31" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="62"/>
+      <c r="C31" s="79"/>
       <c r="D31" s="11"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
@@ -2626,10 +2837,10 @@
       <c r="A34" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="62" t="s">
+      <c r="B34" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="62"/>
+      <c r="C34" s="79"/>
       <c r="D34" s="11"/>
       <c r="E34" s="12"/>
       <c r="F34" s="12"/>
@@ -2738,10 +2949,10 @@
       <c r="A37" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B37" s="62" t="s">
+      <c r="B37" s="79" t="s">
         <v>58</v>
       </c>
-      <c r="C37" s="62"/>
+      <c r="C37" s="79"/>
       <c r="D37" s="11"/>
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
@@ -2948,7 +3159,9 @@
       <c r="Q41" s="3">
         <v>1</v>
       </c>
-      <c r="R41" s="3"/>
+      <c r="R41" s="3">
+        <v>1</v>
+      </c>
       <c r="S41" s="22"/>
       <c r="T41" s="3"/>
       <c r="U41" s="3"/>
@@ -2957,11 +3170,11 @@
       <c r="X41" s="41"/>
       <c r="Y41" s="20">
         <f t="shared" si="2"/>
-        <v>13.5</v>
+        <v>14.5</v>
       </c>
       <c r="Z41" s="20">
         <f t="shared" si="3"/>
-        <v>8.5</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="42" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -3010,7 +3223,9 @@
       <c r="Q42" s="29">
         <v>0.25</v>
       </c>
-      <c r="R42" s="29"/>
+      <c r="R42" s="29">
+        <v>0.25</v>
+      </c>
       <c r="S42" s="30"/>
       <c r="T42" s="29"/>
       <c r="U42" s="29"/>
@@ -3019,21 +3234,21 @@
       <c r="X42" s="39"/>
       <c r="Y42" s="27">
         <f t="shared" si="2"/>
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="Z42" s="27">
         <f t="shared" si="3"/>
-        <v>2.25</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B43" s="62" t="s">
+      <c r="B43" s="79" t="s">
         <v>49</v>
       </c>
-      <c r="C43" s="62"/>
+      <c r="C43" s="79"/>
       <c r="D43" s="11">
         <v>42</v>
       </c>
@@ -3097,11 +3312,11 @@
       <c r="Z44" s="31"/>
     </row>
     <row r="45" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="59" t="s">
+      <c r="A45" s="81" t="s">
         <v>89</v>
       </c>
-      <c r="B45" s="60"/>
-      <c r="C45" s="60"/>
+      <c r="B45" s="82"/>
+      <c r="C45" s="82"/>
       <c r="D45" s="47">
         <f>SUM(D2:D44)</f>
         <v>549</v>
@@ -3156,11 +3371,11 @@
       </c>
       <c r="Q45" s="45">
         <f t="shared" si="4"/>
-        <v>1.25</v>
+        <v>21.25</v>
       </c>
       <c r="R45" s="45">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>26.25</v>
       </c>
       <c r="S45" s="52">
         <f t="shared" si="4"/>
@@ -3188,11 +3403,11 @@
       </c>
       <c r="Y45" s="27">
         <f>SUM(E45:X45)</f>
-        <v>246.75</v>
+        <v>293</v>
       </c>
       <c r="Z45" s="27">
         <f>D45-Y45</f>
-        <v>302.25</v>
+        <v>256</v>
       </c>
     </row>
     <row r="46" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -3224,12 +3439,12 @@
       <c r="Z46" s="14"/>
     </row>
     <row r="47" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="59" t="s">
+      <c r="A47" s="81" t="s">
         <v>99</v>
       </c>
-      <c r="B47" s="60"/>
-      <c r="C47" s="60"/>
-      <c r="D47" s="61"/>
+      <c r="B47" s="82"/>
+      <c r="C47" s="82"/>
+      <c r="D47" s="83"/>
       <c r="E47" s="55">
         <f>($D$45 -12*16-6*40)/(16+6) + 12</f>
         <v>17.31818181818182</v>
@@ -3316,12 +3531,12 @@
       </c>
     </row>
     <row r="48" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="59" t="s">
+      <c r="A48" s="81" t="s">
         <v>100</v>
       </c>
-      <c r="B48" s="60"/>
-      <c r="C48" s="60"/>
-      <c r="D48" s="61"/>
+      <c r="B48" s="82"/>
+      <c r="C48" s="82"/>
+      <c r="D48" s="83"/>
       <c r="E48" s="55">
         <f t="shared" ref="E48:X48" si="7">E47-E45</f>
         <v>9.3181818181818201</v>
@@ -3372,11 +3587,11 @@
       </c>
       <c r="Q48" s="55">
         <f t="shared" si="7"/>
-        <v>16.06818181818182</v>
+        <v>-3.9318181818181799</v>
       </c>
       <c r="R48" s="55">
         <f t="shared" si="7"/>
-        <v>17.31818181818182</v>
+        <v>-8.9318181818181799</v>
       </c>
       <c r="S48" s="55">
         <f t="shared" si="7"/>
@@ -3454,45 +3669,45 @@
       </c>
       <c r="Q49" s="57">
         <f t="shared" ref="Q49" si="10">P49+Q48</f>
-        <v>-21.613636363636338</v>
+        <v>-41.613636363636338</v>
       </c>
       <c r="R49" s="57">
         <f t="shared" ref="R49" si="11">Q49+R48</f>
-        <v>-4.2954545454545183</v>
+        <v>-50.545454545454518</v>
       </c>
       <c r="S49" s="57">
         <f t="shared" ref="S49" si="12">R49+S48</f>
-        <v>41.022727272727302</v>
+        <v>-5.2272727272726982</v>
       </c>
       <c r="T49" s="57">
         <f t="shared" ref="T49" si="13">S49+T48</f>
-        <v>86.340909090909122</v>
+        <v>40.090909090909122</v>
       </c>
       <c r="U49" s="57">
         <f t="shared" ref="U49" si="14">T49+U48</f>
-        <v>131.65909090909093</v>
+        <v>85.409090909090935</v>
       </c>
       <c r="V49" s="57">
         <f t="shared" ref="V49" si="15">U49+V48</f>
-        <v>176.97727272727275</v>
+        <v>130.72727272727275</v>
       </c>
       <c r="W49" s="57">
         <f t="shared" ref="W49" si="16">V49+W48</f>
-        <v>222.29545454545456</v>
+        <v>176.04545454545456</v>
       </c>
       <c r="X49" s="57">
         <f t="shared" ref="X49" si="17">W49+X48</f>
-        <v>267.61363636363637</v>
+        <v>221.36363636363637</v>
+      </c>
+    </row>
+    <row r="53" spans="5:24" x14ac:dyDescent="0.3">
+      <c r="Q53" s="57">
+        <f>SUM(E47:Q47)</f>
+        <v>225.1363636363636</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B17:C17"/>
     <mergeCell ref="A47:D47"/>
     <mergeCell ref="A48:D48"/>
     <mergeCell ref="B31:C31"/>
@@ -3500,14 +3715,1637 @@
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="A45:C45"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B17:C17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="Z2:Z46">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E48:X48">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="Y5" formulaRange="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA520320-61CF-4B89-AD0B-0091112F94A4}">
+  <dimension ref="A1:O51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="Q39" sqref="Q39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.21875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="64.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="13" width="11" style="65" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.5546875" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="80" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="80"/>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="60">
+        <v>44347</v>
+      </c>
+      <c r="F1" s="61">
+        <v>44354</v>
+      </c>
+      <c r="G1" s="61">
+        <v>44361</v>
+      </c>
+      <c r="H1" s="61">
+        <v>44368</v>
+      </c>
+      <c r="I1" s="61">
+        <v>44375</v>
+      </c>
+      <c r="J1" s="61">
+        <v>44382</v>
+      </c>
+      <c r="K1" s="76">
+        <v>44389</v>
+      </c>
+      <c r="L1" s="61">
+        <v>44396</v>
+      </c>
+      <c r="M1" s="75">
+        <v>44403</v>
+      </c>
+      <c r="N1" s="59" t="s">
+        <v>84</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="79" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="79"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="20">
+        <v>5</v>
+      </c>
+      <c r="E3" s="21">
+        <v>5</v>
+      </c>
+      <c r="F3" s="21"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="63"/>
+      <c r="N3" s="24">
+        <f>SUM(E3:M3)</f>
+        <v>5</v>
+      </c>
+      <c r="O3" s="24">
+        <f>D3-N3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="20">
+        <v>5</v>
+      </c>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="63"/>
+      <c r="N4" s="24">
+        <f>SUM(E4:M4)</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="24">
+        <f>D4-N4</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="20">
+        <v>5</v>
+      </c>
+      <c r="E5" s="14"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="70"/>
+      <c r="L5" s="70"/>
+      <c r="M5" s="71"/>
+      <c r="N5" s="24">
+        <f>SUM(F5:M5)</f>
+        <v>0</v>
+      </c>
+      <c r="O5" s="24">
+        <f>D5-N5</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="27">
+        <v>15</v>
+      </c>
+      <c r="E6" s="28">
+        <v>9.5</v>
+      </c>
+      <c r="F6" s="28"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="64"/>
+      <c r="N6" s="24">
+        <f>SUM(E6:M6)</f>
+        <v>9.5</v>
+      </c>
+      <c r="O6" s="24">
+        <f>D6-N6</f>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="79" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="79"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="62"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="11"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="18"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="20">
+        <v>15</v>
+      </c>
+      <c r="E8" s="14">
+        <v>37.5</v>
+      </c>
+      <c r="F8" s="21"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="M8" s="63"/>
+      <c r="N8" s="24">
+        <f>SUM(E8:M8)</f>
+        <v>37.5</v>
+      </c>
+      <c r="O8" s="20">
+        <f>D8-N8</f>
+        <v>-22.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="18"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="20">
+        <v>15</v>
+      </c>
+      <c r="E9" s="14">
+        <v>50.5</v>
+      </c>
+      <c r="F9" s="21"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="58"/>
+      <c r="M9" s="63"/>
+      <c r="N9" s="24">
+        <f>SUM(F9:M9)</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="20">
+        <f>D9-N9</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="25"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="27">
+        <v>15</v>
+      </c>
+      <c r="E10" s="31">
+        <v>31</v>
+      </c>
+      <c r="F10" s="72">
+        <v>1</v>
+      </c>
+      <c r="G10" s="64"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="64"/>
+      <c r="N10" s="24">
+        <f>SUM(E10:M10)</f>
+        <v>32</v>
+      </c>
+      <c r="O10" s="27">
+        <f>D10-N10</f>
+        <v>-17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="79" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="79"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="62"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="24"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="34"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="20">
+        <v>15</v>
+      </c>
+      <c r="E12" s="14">
+        <v>26.5</v>
+      </c>
+      <c r="F12" s="70">
+        <v>1</v>
+      </c>
+      <c r="G12" s="63"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="63"/>
+      <c r="N12" s="24">
+        <f>SUM(E12:M12)</f>
+        <v>27.5</v>
+      </c>
+      <c r="O12" s="24">
+        <f>D12-N12</f>
+        <v>-12.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="34"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="20">
+        <v>8</v>
+      </c>
+      <c r="E13" s="14">
+        <v>28</v>
+      </c>
+      <c r="F13" s="70">
+        <v>5</v>
+      </c>
+      <c r="G13" s="63"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="63"/>
+      <c r="N13" s="24">
+        <f>SUM(E13:M13)</f>
+        <v>33</v>
+      </c>
+      <c r="O13" s="24">
+        <f>D13-N13</f>
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="34"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="20">
+        <v>40</v>
+      </c>
+      <c r="E14" s="14">
+        <v>15</v>
+      </c>
+      <c r="F14" s="70">
+        <v>18</v>
+      </c>
+      <c r="G14" s="71">
+        <v>10</v>
+      </c>
+      <c r="H14" s="21">
+        <v>10</v>
+      </c>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="63"/>
+      <c r="N14" s="24">
+        <f>SUM(E14:M14)</f>
+        <v>53</v>
+      </c>
+      <c r="O14" s="24">
+        <f>D14-N14</f>
+        <v>-13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="34"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="20">
+        <v>5</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="F15" s="70"/>
+      <c r="G15" s="71"/>
+      <c r="H15" s="21">
+        <v>2</v>
+      </c>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="63"/>
+      <c r="N15" s="24">
+        <f>SUM(E15:M15)</f>
+        <v>2</v>
+      </c>
+      <c r="O15" s="24">
+        <f>D15-N15</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="25"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="27">
+        <v>5</v>
+      </c>
+      <c r="E16" s="31"/>
+      <c r="F16" s="72"/>
+      <c r="G16" s="73"/>
+      <c r="H16" s="28">
+        <v>5</v>
+      </c>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="64"/>
+      <c r="N16" s="74">
+        <f>SUM(E16:M16)</f>
+        <v>5</v>
+      </c>
+      <c r="O16" s="24">
+        <f>D16-N16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="79" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="79"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="37"/>
+      <c r="M17" s="62"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="11"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="20">
+        <v>3</v>
+      </c>
+      <c r="E18" s="14">
+        <v>6</v>
+      </c>
+      <c r="F18" s="21"/>
+      <c r="G18" s="63"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="63"/>
+      <c r="N18" s="24">
+        <f>SUM(E18:M18)</f>
+        <v>6</v>
+      </c>
+      <c r="O18" s="20">
+        <f>D18-N18</f>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="20">
+        <v>10</v>
+      </c>
+      <c r="E19" s="14">
+        <v>10</v>
+      </c>
+      <c r="F19" s="21"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="63"/>
+      <c r="N19" s="24">
+        <f>SUM(E19:M19)</f>
+        <v>10</v>
+      </c>
+      <c r="O19" s="20">
+        <f>D19-N19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="27">
+        <v>5</v>
+      </c>
+      <c r="E20" s="31"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="73"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="64"/>
+      <c r="N20" s="24">
+        <f>SUM(E20:M20)</f>
+        <v>0</v>
+      </c>
+      <c r="O20" s="20">
+        <f>D20-N20</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" s="84"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="63"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="63"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="17"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="35"/>
+      <c r="C22" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="D22" s="20">
+        <v>25</v>
+      </c>
+      <c r="E22" s="14"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="63"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="70"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="21">
+        <v>20</v>
+      </c>
+      <c r="L22" s="21">
+        <v>5</v>
+      </c>
+      <c r="M22" s="63"/>
+      <c r="N22" s="24">
+        <f t="shared" ref="N22:N27" si="0">SUM(E22:M22)</f>
+        <v>25</v>
+      </c>
+      <c r="O22" s="24">
+        <f t="shared" ref="O22:O32" si="1">D22-N22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="35"/>
+      <c r="C23" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" s="20">
+        <v>1</v>
+      </c>
+      <c r="E23" s="14"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="63"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="70"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="21">
+        <v>1</v>
+      </c>
+      <c r="M23" s="63"/>
+      <c r="N23" s="24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O23" s="24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24" s="35"/>
+      <c r="C24" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" s="20">
+        <v>5</v>
+      </c>
+      <c r="E24" s="14"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="63"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="70"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21">
+        <v>1</v>
+      </c>
+      <c r="M24" s="63"/>
+      <c r="N24" s="24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O24" s="24">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="35"/>
+      <c r="C25" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" s="20">
+        <v>5</v>
+      </c>
+      <c r="E25" s="14"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="63"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="70"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="63"/>
+      <c r="N25" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O25" s="24">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B26" s="35"/>
+      <c r="C26" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="D26" s="20">
+        <v>5</v>
+      </c>
+      <c r="E26" s="14"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="63"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="70"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="28"/>
+      <c r="L26" s="21"/>
+      <c r="M26" s="63"/>
+      <c r="N26" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O26" s="24">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="79" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="79"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="62"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="37"/>
+      <c r="M27" s="62"/>
+      <c r="N27" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O27" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A28" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B28" s="35"/>
+      <c r="C28" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" s="20">
+        <v>15</v>
+      </c>
+      <c r="E28" s="14"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="63"/>
+      <c r="H28" s="21">
+        <v>5</v>
+      </c>
+      <c r="I28" s="65">
+        <v>3</v>
+      </c>
+      <c r="J28" s="70"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="21"/>
+      <c r="M28" s="63"/>
+      <c r="N28" s="24">
+        <f t="shared" ref="N28:N34" si="2">SUM(E28:M28)</f>
+        <v>8</v>
+      </c>
+      <c r="O28" s="24">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A29" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="B29" s="35"/>
+      <c r="C29" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="D29" s="20">
+        <v>10</v>
+      </c>
+      <c r="E29" s="14"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="63"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="65">
+        <v>2</v>
+      </c>
+      <c r="J29" s="70"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="21"/>
+      <c r="M29" s="63"/>
+      <c r="N29" s="24">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="O29" s="24">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="B30" s="35"/>
+      <c r="C30" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="D30" s="20">
+        <v>5</v>
+      </c>
+      <c r="E30" s="14"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="63"/>
+      <c r="H30" s="21"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="70"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="63"/>
+      <c r="N30" s="24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O30" s="24">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B31" s="35"/>
+      <c r="C31" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D31" s="20">
+        <v>10</v>
+      </c>
+      <c r="E31" s="14"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="63"/>
+      <c r="H31" s="21"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="78"/>
+      <c r="L31" s="21"/>
+      <c r="M31" s="63"/>
+      <c r="N31" s="24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O31" s="24">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B32" s="35"/>
+      <c r="C32" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="D32" s="20">
+        <v>10</v>
+      </c>
+      <c r="E32" s="14"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="21"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="78"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="63"/>
+      <c r="N32" s="24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O32" s="24">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A33" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B33" s="35"/>
+      <c r="C33" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="D33" s="20">
+        <v>25</v>
+      </c>
+      <c r="E33" s="14"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="63"/>
+      <c r="H33" s="21"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="38"/>
+      <c r="L33" s="70"/>
+      <c r="M33" s="63"/>
+      <c r="N33" s="24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O33" s="24">
+        <f t="shared" ref="O33:O34" si="3">D33-N33</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B34" s="35"/>
+      <c r="C34" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="D34" s="20">
+        <v>10</v>
+      </c>
+      <c r="E34" s="14"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="63"/>
+      <c r="H34" s="21"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="28"/>
+      <c r="L34" s="70"/>
+      <c r="M34" s="71"/>
+      <c r="N34" s="24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O34" s="24">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A35" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="79" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" s="79"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="37"/>
+      <c r="G35" s="62"/>
+      <c r="H35" s="37"/>
+      <c r="I35" s="37"/>
+      <c r="J35" s="37"/>
+      <c r="K35" s="21"/>
+      <c r="L35" s="37"/>
+      <c r="M35" s="62"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="20"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A36" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="20">
+        <v>50</v>
+      </c>
+      <c r="E36" s="14"/>
+      <c r="F36" s="70"/>
+      <c r="G36" s="71"/>
+      <c r="H36" s="70"/>
+      <c r="I36" s="70">
+        <v>28</v>
+      </c>
+      <c r="J36" s="70">
+        <v>35</v>
+      </c>
+      <c r="K36" s="70">
+        <v>22</v>
+      </c>
+      <c r="L36" s="70">
+        <v>20</v>
+      </c>
+      <c r="M36" s="71">
+        <v>15</v>
+      </c>
+      <c r="N36" s="14">
+        <f>SUM(E36:M36)</f>
+        <v>120</v>
+      </c>
+      <c r="O36" s="20">
+        <f>D36-N36</f>
+        <v>-70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="27">
+        <v>10</v>
+      </c>
+      <c r="E37" s="31"/>
+      <c r="F37" s="72"/>
+      <c r="G37" s="73"/>
+      <c r="H37" s="72"/>
+      <c r="I37" s="72">
+        <v>5</v>
+      </c>
+      <c r="J37" s="72"/>
+      <c r="K37" s="72"/>
+      <c r="L37" s="72"/>
+      <c r="M37" s="73"/>
+      <c r="N37" s="31">
+        <f>SUM(E37:M37)</f>
+        <v>5</v>
+      </c>
+      <c r="O37" s="27">
+        <f>D37-N37</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A38" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38" s="79" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" s="79"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="62"/>
+      <c r="H38" s="37"/>
+      <c r="I38" s="37"/>
+      <c r="J38" s="37"/>
+      <c r="K38" s="21"/>
+      <c r="L38" s="37"/>
+      <c r="M38" s="62"/>
+      <c r="N38" s="24"/>
+      <c r="O38" s="20"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A39" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="20">
+        <v>3</v>
+      </c>
+      <c r="E39" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="F39" s="21"/>
+      <c r="G39" s="63"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="21"/>
+      <c r="J39" s="21"/>
+      <c r="K39" s="21"/>
+      <c r="L39" s="21"/>
+      <c r="M39" s="63"/>
+      <c r="N39" s="24">
+        <f t="shared" ref="N39:N45" si="4">SUM(E39:M39)</f>
+        <v>0.5</v>
+      </c>
+      <c r="O39" s="20">
+        <f t="shared" ref="O39:O45" si="5">D39-N39</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A40" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="35"/>
+      <c r="C40" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D40" s="20">
+        <v>10</v>
+      </c>
+      <c r="E40" s="21">
+        <v>14.5</v>
+      </c>
+      <c r="G40" s="63"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="21"/>
+      <c r="K40" s="21"/>
+      <c r="L40" s="21"/>
+      <c r="M40" s="63"/>
+      <c r="N40" s="24">
+        <f t="shared" si="4"/>
+        <v>14.5</v>
+      </c>
+      <c r="O40" s="20">
+        <f t="shared" si="5"/>
+        <v>-4.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A41" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" s="19"/>
+      <c r="C41" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="D41" s="20">
+        <v>2</v>
+      </c>
+      <c r="E41" s="21">
+        <v>1.5</v>
+      </c>
+      <c r="F41" s="77">
+        <v>1</v>
+      </c>
+      <c r="G41" s="63"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="21"/>
+      <c r="L41" s="21"/>
+      <c r="M41" s="63"/>
+      <c r="N41" s="24">
+        <f t="shared" si="4"/>
+        <v>2.5</v>
+      </c>
+      <c r="O41" s="20">
+        <f t="shared" si="5"/>
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A42" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="D42" s="20">
+        <v>22</v>
+      </c>
+      <c r="E42" s="21">
+        <v>13.5</v>
+      </c>
+      <c r="F42" s="77">
+        <v>1</v>
+      </c>
+      <c r="G42" s="71"/>
+      <c r="H42" s="70">
+        <v>1</v>
+      </c>
+      <c r="I42" s="70">
+        <v>1</v>
+      </c>
+      <c r="J42" s="70">
+        <v>1</v>
+      </c>
+      <c r="K42" s="70">
+        <v>1</v>
+      </c>
+      <c r="L42" s="70">
+        <v>1</v>
+      </c>
+      <c r="M42" s="71"/>
+      <c r="N42" s="24">
+        <f t="shared" si="4"/>
+        <v>19.5</v>
+      </c>
+      <c r="O42" s="20">
+        <f t="shared" si="5"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="B43" s="26"/>
+      <c r="C43" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="D43" s="27">
+        <v>5</v>
+      </c>
+      <c r="E43" s="31">
+        <v>2.75</v>
+      </c>
+      <c r="F43" s="72">
+        <v>0.25</v>
+      </c>
+      <c r="G43" s="73"/>
+      <c r="H43" s="72">
+        <v>0.25</v>
+      </c>
+      <c r="I43" s="72">
+        <v>0.25</v>
+      </c>
+      <c r="J43" s="72">
+        <v>0.25</v>
+      </c>
+      <c r="K43" s="72">
+        <v>0.25</v>
+      </c>
+      <c r="L43" s="72">
+        <v>0.25</v>
+      </c>
+      <c r="M43" s="73"/>
+      <c r="N43" s="74">
+        <f t="shared" si="4"/>
+        <v>4.25</v>
+      </c>
+      <c r="O43" s="27">
+        <f t="shared" si="5"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B44" s="80" t="s">
+        <v>124</v>
+      </c>
+      <c r="C44" s="85"/>
+      <c r="D44" s="20">
+        <v>10</v>
+      </c>
+      <c r="E44" s="14"/>
+      <c r="F44" s="70">
+        <v>8</v>
+      </c>
+      <c r="G44" s="71">
+        <v>1</v>
+      </c>
+      <c r="H44" s="21"/>
+      <c r="I44" s="21"/>
+      <c r="J44" s="21"/>
+      <c r="K44" s="28"/>
+      <c r="L44" s="21"/>
+      <c r="M44" s="63"/>
+      <c r="N44" s="74">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="O44" s="27">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B45" s="79" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" s="79"/>
+      <c r="D45" s="11">
+        <v>42</v>
+      </c>
+      <c r="E45" s="12">
+        <v>10</v>
+      </c>
+      <c r="F45" s="37"/>
+      <c r="G45" s="62"/>
+      <c r="H45" s="37"/>
+      <c r="I45" s="37"/>
+      <c r="J45" s="37"/>
+      <c r="K45" s="66"/>
+      <c r="L45" s="37">
+        <v>12</v>
+      </c>
+      <c r="M45" s="62">
+        <v>15</v>
+      </c>
+      <c r="N45" s="48">
+        <f t="shared" si="4"/>
+        <v>37</v>
+      </c>
+      <c r="O45" s="48">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="49"/>
+      <c r="B46" s="50"/>
+      <c r="C46" s="50"/>
+      <c r="D46" s="45"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="37"/>
+      <c r="G46" s="62"/>
+      <c r="H46" s="37"/>
+      <c r="I46" s="37"/>
+      <c r="J46" s="37"/>
+      <c r="K46" s="66"/>
+      <c r="L46" s="37"/>
+      <c r="M46" s="62"/>
+      <c r="N46" s="31"/>
+      <c r="O46" s="31"/>
+    </row>
+    <row r="47" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="81" t="s">
+        <v>89</v>
+      </c>
+      <c r="B47" s="82"/>
+      <c r="C47" s="82"/>
+      <c r="D47" s="47">
+        <f>SUM(D2:D46)</f>
+        <v>446</v>
+      </c>
+      <c r="E47" s="45">
+        <f t="shared" ref="E47:M47" si="6">SUM(E2:E45)</f>
+        <v>261.75</v>
+      </c>
+      <c r="F47" s="66">
+        <f t="shared" si="6"/>
+        <v>35.25</v>
+      </c>
+      <c r="G47" s="67">
+        <f t="shared" si="6"/>
+        <v>11</v>
+      </c>
+      <c r="H47" s="66">
+        <f t="shared" si="6"/>
+        <v>23.25</v>
+      </c>
+      <c r="I47" s="66">
+        <f t="shared" si="6"/>
+        <v>39.25</v>
+      </c>
+      <c r="J47" s="66">
+        <f t="shared" si="6"/>
+        <v>36.25</v>
+      </c>
+      <c r="K47" s="66">
+        <f t="shared" si="6"/>
+        <v>43.25</v>
+      </c>
+      <c r="L47" s="66">
+        <f t="shared" si="6"/>
+        <v>40.25</v>
+      </c>
+      <c r="M47" s="67">
+        <f t="shared" si="6"/>
+        <v>30</v>
+      </c>
+      <c r="N47" s="74">
+        <f>SUM(E47:M47)</f>
+        <v>520.25</v>
+      </c>
+      <c r="O47" s="27">
+        <f>D47-N47</f>
+        <v>-74.25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="54"/>
+      <c r="B48" s="54"/>
+      <c r="C48" s="54"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="45"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="21"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="21"/>
+      <c r="J48" s="21"/>
+      <c r="K48" s="21"/>
+      <c r="L48" s="21"/>
+      <c r="M48" s="21"/>
+      <c r="N48" s="14"/>
+      <c r="O48" s="14"/>
+    </row>
+    <row r="49" spans="1:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="81" t="s">
+        <v>99</v>
+      </c>
+      <c r="B49" s="82"/>
+      <c r="C49" s="82"/>
+      <c r="D49" s="83"/>
+      <c r="E49" s="57">
+        <v>261.75</v>
+      </c>
+      <c r="F49" s="68">
+        <v>15</v>
+      </c>
+      <c r="G49" s="68">
+        <v>15</v>
+      </c>
+      <c r="H49" s="68">
+        <v>40</v>
+      </c>
+      <c r="I49" s="68">
+        <v>40</v>
+      </c>
+      <c r="J49" s="68">
+        <v>40</v>
+      </c>
+      <c r="K49" s="68">
+        <v>40</v>
+      </c>
+      <c r="L49" s="68">
+        <v>40</v>
+      </c>
+      <c r="M49" s="68">
+        <v>40</v>
+      </c>
+      <c r="N49" s="57">
+        <f>SUM(E49:M49)</f>
+        <v>531.75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="81" t="s">
+        <v>100</v>
+      </c>
+      <c r="B50" s="82"/>
+      <c r="C50" s="82"/>
+      <c r="D50" s="83"/>
+      <c r="E50" s="55">
+        <f t="shared" ref="E50:M50" si="7">E49-E47</f>
+        <v>0</v>
+      </c>
+      <c r="F50" s="68">
+        <f t="shared" si="7"/>
+        <v>-20.25</v>
+      </c>
+      <c r="G50" s="68">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="H50" s="68">
+        <f t="shared" si="7"/>
+        <v>16.75</v>
+      </c>
+      <c r="I50" s="68">
+        <f t="shared" si="7"/>
+        <v>0.75</v>
+      </c>
+      <c r="J50" s="68">
+        <f t="shared" si="7"/>
+        <v>3.75</v>
+      </c>
+      <c r="K50" s="68">
+        <f t="shared" si="7"/>
+        <v>-3.25</v>
+      </c>
+      <c r="L50" s="68">
+        <f t="shared" si="7"/>
+        <v>-0.25</v>
+      </c>
+      <c r="M50" s="68">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E51" s="57">
+        <f>D51+E50</f>
+        <v>0</v>
+      </c>
+      <c r="F51" s="69">
+        <f>E51+F50</f>
+        <v>-20.25</v>
+      </c>
+      <c r="G51" s="57">
+        <f t="shared" ref="G51:M51" si="8">F51+G50</f>
+        <v>-16.25</v>
+      </c>
+      <c r="H51" s="69">
+        <f t="shared" si="8"/>
+        <v>0.5</v>
+      </c>
+      <c r="I51" s="57">
+        <f t="shared" si="8"/>
+        <v>1.25</v>
+      </c>
+      <c r="J51" s="69">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="K51" s="57">
+        <f t="shared" si="8"/>
+        <v>1.75</v>
+      </c>
+      <c r="L51" s="69">
+        <f t="shared" si="8"/>
+        <v>1.5</v>
+      </c>
+      <c r="M51" s="57">
+        <f t="shared" si="8"/>
+        <v>11.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B17:C17"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="O2:O48">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E50:M50">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3517,8 +5355,5 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="Y5" formulaRange="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>